<commit_message>
chome driver update selenium
</commit_message>
<xml_diff>
--- a/Dumps/iexDamFile/MarketMinute.xlsx
+++ b/Dumps/iexDamFile/MarketMinute.xlsx
@@ -386,7 +386,7 @@
     <row r="4" ht="14.4" customHeight="1">
       <c s="2" t="inlineStr" r="A4">
         <is>
-          <t xml:space="preserve">Date: 01-03-2021</t>
+          <t xml:space="preserve">Date: 24-03-2021</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
     <row r="7" ht="13.6" customHeight="0">
       <c s="6" t="inlineStr" r="A7">
         <is>
-          <t xml:space="preserve">01-03-2021</t>
+          <t xml:space="preserve">24-03-2021</t>
         </is>
       </c>
       <c s="7" r="B7">
@@ -474,22 +474,22 @@
       </c>
       <c s="9" t="inlineStr" r="D7">
         <is>
-          <t xml:space="preserve">8277.70</t>
+          <t xml:space="preserve">11531.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F7">
         <is>
-          <t xml:space="preserve">10873.60</t>
+          <t xml:space="preserve">10686.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G7">
         <is>
-          <t xml:space="preserve">6395.20</t>
+          <t xml:space="preserve">9085.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H7">
         <is>
-          <t xml:space="preserve">6430.60</t>
+          <t xml:space="preserve">9073.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I7">
@@ -499,12 +499,12 @@
       </c>
       <c s="9" t="inlineStr" r="J7">
         <is>
-          <t xml:space="preserve">6430.60</t>
+          <t xml:space="preserve">9073.40</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K7">
         <is>
-          <t xml:space="preserve">3429.15</t>
+          <t xml:space="preserve">4129.37</t>
         </is>
       </c>
     </row>
@@ -518,22 +518,22 @@
       </c>
       <c s="9" t="inlineStr" r="D8">
         <is>
-          <t xml:space="preserve">8295.90</t>
+          <t xml:space="preserve">12067.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F8">
         <is>
-          <t xml:space="preserve">11689.10</t>
+          <t xml:space="preserve">10869.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G8">
         <is>
-          <t xml:space="preserve">6453.80</t>
+          <t xml:space="preserve">9567.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H8">
         <is>
-          <t xml:space="preserve">6459.50</t>
+          <t xml:space="preserve">9553.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I8">
@@ -543,12 +543,12 @@
       </c>
       <c s="9" t="inlineStr" r="J8">
         <is>
-          <t xml:space="preserve">6459.50</t>
+          <t xml:space="preserve">9553.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K8">
         <is>
-          <t xml:space="preserve">3294.73</t>
+          <t xml:space="preserve">4382.34</t>
         </is>
       </c>
     </row>
@@ -562,22 +562,22 @@
       </c>
       <c s="9" t="inlineStr" r="D9">
         <is>
-          <t xml:space="preserve">8270.40</t>
+          <t xml:space="preserve">12139.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F9">
         <is>
-          <t xml:space="preserve">12789.20</t>
+          <t xml:space="preserve">11751.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G9">
         <is>
-          <t xml:space="preserve">6428.40</t>
+          <t xml:space="preserve">9884.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H9">
         <is>
-          <t xml:space="preserve">6451.00</t>
+          <t xml:space="preserve">9884.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I9">
@@ -587,12 +587,12 @@
       </c>
       <c s="9" t="inlineStr" r="J9">
         <is>
-          <t xml:space="preserve">6451.00</t>
+          <t xml:space="preserve">9884.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K9">
         <is>
-          <t xml:space="preserve">3294.23</t>
+          <t xml:space="preserve">3666.62</t>
         </is>
       </c>
     </row>
@@ -606,22 +606,22 @@
       </c>
       <c s="9" t="inlineStr" r="D10">
         <is>
-          <t xml:space="preserve">8337.50</t>
+          <t xml:space="preserve">12133.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F10">
         <is>
-          <t xml:space="preserve">13161.20</t>
+          <t xml:space="preserve">12099.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G10">
         <is>
-          <t xml:space="preserve">6454.70</t>
+          <t xml:space="preserve">10020.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H10">
         <is>
-          <t xml:space="preserve">6503.40</t>
+          <t xml:space="preserve">10007.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I10">
@@ -631,12 +631,12 @@
       </c>
       <c s="9" t="inlineStr" r="J10">
         <is>
-          <t xml:space="preserve">6503.40</t>
+          <t xml:space="preserve">10007.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K10">
         <is>
-          <t xml:space="preserve">3229.53</t>
+          <t xml:space="preserve">3549.79</t>
         </is>
       </c>
     </row>
@@ -652,22 +652,22 @@
       </c>
       <c s="9" t="inlineStr" r="D11">
         <is>
-          <t xml:space="preserve">8254.10</t>
+          <t xml:space="preserve">11985.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F11">
         <is>
-          <t xml:space="preserve">13863.90</t>
+          <t xml:space="preserve">12895.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G11">
         <is>
-          <t xml:space="preserve">6489.20</t>
+          <t xml:space="preserve">10347.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H11">
         <is>
-          <t xml:space="preserve">6573.90</t>
+          <t xml:space="preserve">10347.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I11">
@@ -677,12 +677,12 @@
       </c>
       <c s="9" t="inlineStr" r="J11">
         <is>
-          <t xml:space="preserve">6573.90</t>
+          <t xml:space="preserve">10347.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K11">
         <is>
-          <t xml:space="preserve">3113.47</t>
+          <t xml:space="preserve">3444.06</t>
         </is>
       </c>
     </row>
@@ -696,22 +696,22 @@
       </c>
       <c s="9" t="inlineStr" r="D12">
         <is>
-          <t xml:space="preserve">8115.70</t>
+          <t xml:space="preserve">11836.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F12">
         <is>
-          <t xml:space="preserve">14267.90</t>
+          <t xml:space="preserve">13377.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G12">
         <is>
-          <t xml:space="preserve">6467.70</t>
+          <t xml:space="preserve">10293.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H12">
         <is>
-          <t xml:space="preserve">6470.10</t>
+          <t xml:space="preserve">10282.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I12">
@@ -721,12 +721,12 @@
       </c>
       <c s="9" t="inlineStr" r="J12">
         <is>
-          <t xml:space="preserve">6470.10</t>
+          <t xml:space="preserve">10282.40</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K12">
         <is>
-          <t xml:space="preserve">3027.90</t>
+          <t xml:space="preserve">3359.30</t>
         </is>
       </c>
     </row>
@@ -740,22 +740,22 @@
       </c>
       <c s="9" t="inlineStr" r="D13">
         <is>
-          <t xml:space="preserve">8052.80</t>
+          <t xml:space="preserve">11910.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F13">
         <is>
-          <t xml:space="preserve">14670.80</t>
+          <t xml:space="preserve">14106.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G13">
         <is>
-          <t xml:space="preserve">6405.00</t>
+          <t xml:space="preserve">10418.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H13">
         <is>
-          <t xml:space="preserve">6433.60</t>
+          <t xml:space="preserve">10407.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I13">
@@ -765,12 +765,12 @@
       </c>
       <c s="9" t="inlineStr" r="J13">
         <is>
-          <t xml:space="preserve">6433.60</t>
+          <t xml:space="preserve">10407.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K13">
         <is>
-          <t xml:space="preserve">3027.31</t>
+          <t xml:space="preserve">3279.00</t>
         </is>
       </c>
     </row>
@@ -784,22 +784,22 @@
       </c>
       <c s="9" t="inlineStr" r="D14">
         <is>
-          <t xml:space="preserve">7971.20</t>
+          <t xml:space="preserve">11766.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F14">
         <is>
-          <t xml:space="preserve">14981.90</t>
+          <t xml:space="preserve">14345.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G14">
         <is>
-          <t xml:space="preserve">6348.70</t>
+          <t xml:space="preserve">10347.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H14">
         <is>
-          <t xml:space="preserve">6403.10</t>
+          <t xml:space="preserve">10336.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I14">
@@ -809,12 +809,12 @@
       </c>
       <c s="9" t="inlineStr" r="J14">
         <is>
-          <t xml:space="preserve">6403.10</t>
+          <t xml:space="preserve">10336.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K14">
         <is>
-          <t xml:space="preserve">3000.73</t>
+          <t xml:space="preserve">3143.88</t>
         </is>
       </c>
     </row>
@@ -830,22 +830,22 @@
       </c>
       <c s="9" t="inlineStr" r="D15">
         <is>
-          <t xml:space="preserve">7960.80</t>
+          <t xml:space="preserve">11942.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F15">
         <is>
-          <t xml:space="preserve">15566.20</t>
+          <t xml:space="preserve">14541.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G15">
         <is>
-          <t xml:space="preserve">6416.70</t>
+          <t xml:space="preserve">10563.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H15">
         <is>
-          <t xml:space="preserve">6419.10</t>
+          <t xml:space="preserve">10550.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I15">
@@ -855,12 +855,12 @@
       </c>
       <c s="9" t="inlineStr" r="J15">
         <is>
-          <t xml:space="preserve">6419.10</t>
+          <t xml:space="preserve">10550.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K15">
         <is>
-          <t xml:space="preserve">2959.07</t>
+          <t xml:space="preserve">3199.43</t>
         </is>
       </c>
     </row>
@@ -874,22 +874,22 @@
       </c>
       <c s="9" t="inlineStr" r="D16">
         <is>
-          <t xml:space="preserve">7938.50</t>
+          <t xml:space="preserve">11868.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F16">
         <is>
-          <t xml:space="preserve">15729.10</t>
+          <t xml:space="preserve">14521.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G16">
         <is>
-          <t xml:space="preserve">6394.60</t>
+          <t xml:space="preserve">10490.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H16">
         <is>
-          <t xml:space="preserve">6406.00</t>
+          <t xml:space="preserve">10476.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I16">
@@ -899,12 +899,12 @@
       </c>
       <c s="9" t="inlineStr" r="J16">
         <is>
-          <t xml:space="preserve">6406.00</t>
+          <t xml:space="preserve">10476.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K16">
         <is>
-          <t xml:space="preserve">2947.20</t>
+          <t xml:space="preserve">3199.56</t>
         </is>
       </c>
     </row>
@@ -918,22 +918,22 @@
       </c>
       <c s="9" t="inlineStr" r="D17">
         <is>
-          <t xml:space="preserve">7852.00</t>
+          <t xml:space="preserve">11828.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F17">
         <is>
-          <t xml:space="preserve">15755.80</t>
+          <t xml:space="preserve">14671.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G17">
         <is>
-          <t xml:space="preserve">6317.50</t>
+          <t xml:space="preserve">10450.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H17">
         <is>
-          <t xml:space="preserve">6319.90</t>
+          <t xml:space="preserve">10440.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I17">
@@ -943,12 +943,12 @@
       </c>
       <c s="9" t="inlineStr" r="J17">
         <is>
-          <t xml:space="preserve">6319.90</t>
+          <t xml:space="preserve">10440.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K17">
         <is>
-          <t xml:space="preserve">2889.07</t>
+          <t xml:space="preserve">3192.09</t>
         </is>
       </c>
     </row>
@@ -962,22 +962,22 @@
       </c>
       <c s="9" t="inlineStr" r="D18">
         <is>
-          <t xml:space="preserve">7872.30</t>
+          <t xml:space="preserve">11389.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F18">
         <is>
-          <t xml:space="preserve">16023.80</t>
+          <t xml:space="preserve">14807.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G18">
         <is>
-          <t xml:space="preserve">6338.20</t>
+          <t xml:space="preserve">10061.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H18">
         <is>
-          <t xml:space="preserve">6361.60</t>
+          <t xml:space="preserve">10048.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I18">
@@ -987,12 +987,12 @@
       </c>
       <c s="9" t="inlineStr" r="J18">
         <is>
-          <t xml:space="preserve">6361.60</t>
+          <t xml:space="preserve">10048.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K18">
         <is>
-          <t xml:space="preserve">2883.07</t>
+          <t xml:space="preserve">3085.11</t>
         </is>
       </c>
     </row>
@@ -1008,22 +1008,22 @@
       </c>
       <c s="9" t="inlineStr" r="D19">
         <is>
-          <t xml:space="preserve">8221.50</t>
+          <t xml:space="preserve">11425.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F19">
         <is>
-          <t xml:space="preserve">15840.80</t>
+          <t xml:space="preserve">15234.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G19">
         <is>
-          <t xml:space="preserve">6682.80</t>
+          <t xml:space="preserve">10127.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H19">
         <is>
-          <t xml:space="preserve">6685.20</t>
+          <t xml:space="preserve">10114.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I19">
@@ -1033,12 +1033,12 @@
       </c>
       <c s="9" t="inlineStr" r="J19">
         <is>
-          <t xml:space="preserve">6685.20</t>
+          <t xml:space="preserve">10114.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K19">
         <is>
-          <t xml:space="preserve">2899.94</t>
+          <t xml:space="preserve">3059.98</t>
         </is>
       </c>
     </row>
@@ -1052,22 +1052,22 @@
       </c>
       <c s="9" t="inlineStr" r="D20">
         <is>
-          <t xml:space="preserve">8219.70</t>
+          <t xml:space="preserve">11299.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F20">
         <is>
-          <t xml:space="preserve">15690.80</t>
+          <t xml:space="preserve">15281.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G20">
         <is>
-          <t xml:space="preserve">6680.60</t>
+          <t xml:space="preserve">10000.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H20">
         <is>
-          <t xml:space="preserve">6683.00</t>
+          <t xml:space="preserve">9987.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I20">
@@ -1077,12 +1077,12 @@
       </c>
       <c s="9" t="inlineStr" r="J20">
         <is>
-          <t xml:space="preserve">6683.00</t>
+          <t xml:space="preserve">9987.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K20">
         <is>
-          <t xml:space="preserve">2891.41</t>
+          <t xml:space="preserve">3059.72</t>
         </is>
       </c>
     </row>
@@ -1096,22 +1096,22 @@
       </c>
       <c s="9" t="inlineStr" r="D21">
         <is>
-          <t xml:space="preserve">8276.60</t>
+          <t xml:space="preserve">11196.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F21">
         <is>
-          <t xml:space="preserve">15434.80</t>
+          <t xml:space="preserve">15440.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G21">
         <is>
-          <t xml:space="preserve">6737.20</t>
+          <t xml:space="preserve">9897.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H21">
         <is>
-          <t xml:space="preserve">6739.60</t>
+          <t xml:space="preserve">9884.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I21">
@@ -1121,12 +1121,12 @@
       </c>
       <c s="9" t="inlineStr" r="J21">
         <is>
-          <t xml:space="preserve">6739.60</t>
+          <t xml:space="preserve">9884.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K21">
         <is>
-          <t xml:space="preserve">2889.93</t>
+          <t xml:space="preserve">3059.32</t>
         </is>
       </c>
     </row>
@@ -1140,22 +1140,22 @@
       </c>
       <c s="9" t="inlineStr" r="D22">
         <is>
-          <t xml:space="preserve">8205.00</t>
+          <t xml:space="preserve">11150.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F22">
         <is>
-          <t xml:space="preserve">15902.80</t>
+          <t xml:space="preserve">15480.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G22">
         <is>
-          <t xml:space="preserve">6665.30</t>
+          <t xml:space="preserve">9851.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H22">
         <is>
-          <t xml:space="preserve">6667.70</t>
+          <t xml:space="preserve">9838.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I22">
@@ -1165,12 +1165,12 @@
       </c>
       <c s="9" t="inlineStr" r="J22">
         <is>
-          <t xml:space="preserve">6667.70</t>
+          <t xml:space="preserve">9838.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K22">
         <is>
-          <t xml:space="preserve">2890.50</t>
+          <t xml:space="preserve">3059.17</t>
         </is>
       </c>
     </row>
@@ -1186,22 +1186,22 @@
       </c>
       <c s="9" t="inlineStr" r="D23">
         <is>
-          <t xml:space="preserve">8607.70</t>
+          <t xml:space="preserve">11311.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F23">
         <is>
-          <t xml:space="preserve">15095.80</t>
+          <t xml:space="preserve">15830.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G23">
         <is>
-          <t xml:space="preserve">6865.30</t>
+          <t xml:space="preserve">10009.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H23">
         <is>
-          <t xml:space="preserve">6888.70</t>
+          <t xml:space="preserve">9996.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I23">
@@ -1211,12 +1211,12 @@
       </c>
       <c s="9" t="inlineStr" r="J23">
         <is>
-          <t xml:space="preserve">6888.70</t>
+          <t xml:space="preserve">9996.40</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K23">
         <is>
-          <t xml:space="preserve">2886.50</t>
+          <t xml:space="preserve">3049.48</t>
         </is>
       </c>
     </row>
@@ -1230,22 +1230,22 @@
       </c>
       <c s="9" t="inlineStr" r="D24">
         <is>
-          <t xml:space="preserve">8950.60</t>
+          <t xml:space="preserve">12006.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F24">
         <is>
-          <t xml:space="preserve">14549.00</t>
+          <t xml:space="preserve">15670.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G24">
         <is>
-          <t xml:space="preserve">7204.40</t>
+          <t xml:space="preserve">10678.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H24">
         <is>
-          <t xml:space="preserve">7206.80</t>
+          <t xml:space="preserve">10665.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I24">
@@ -1255,12 +1255,12 @@
       </c>
       <c s="9" t="inlineStr" r="J24">
         <is>
-          <t xml:space="preserve">7206.80</t>
+          <t xml:space="preserve">10665.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K24">
         <is>
-          <t xml:space="preserve">2959.84</t>
+          <t xml:space="preserve">3085.17</t>
         </is>
       </c>
     </row>
@@ -1274,22 +1274,22 @@
       </c>
       <c s="9" t="inlineStr" r="D25">
         <is>
-          <t xml:space="preserve">8887.60</t>
+          <t xml:space="preserve">12176.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F25">
         <is>
-          <t xml:space="preserve">14040.50</t>
+          <t xml:space="preserve">15742.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G25">
         <is>
-          <t xml:space="preserve">7065.60</t>
+          <t xml:space="preserve">10852.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H25">
         <is>
-          <t xml:space="preserve">7145.40</t>
+          <t xml:space="preserve">10826.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I25">
@@ -1299,12 +1299,12 @@
       </c>
       <c s="9" t="inlineStr" r="J25">
         <is>
-          <t xml:space="preserve">7145.40</t>
+          <t xml:space="preserve">10826.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K25">
         <is>
-          <t xml:space="preserve">3027.13</t>
+          <t xml:space="preserve">3085.91</t>
         </is>
       </c>
     </row>
@@ -1318,22 +1318,22 @@
       </c>
       <c s="9" t="inlineStr" r="D26">
         <is>
-          <t xml:space="preserve">9043.60</t>
+          <t xml:space="preserve">12282.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F26">
         <is>
-          <t xml:space="preserve">13515.60</t>
+          <t xml:space="preserve">15368.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G26">
         <is>
-          <t xml:space="preserve">7154.30</t>
+          <t xml:space="preserve">10914.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H26">
         <is>
-          <t xml:space="preserve">7223.90</t>
+          <t xml:space="preserve">10893.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I26">
@@ -1343,12 +1343,12 @@
       </c>
       <c s="9" t="inlineStr" r="J26">
         <is>
-          <t xml:space="preserve">7223.90</t>
+          <t xml:space="preserve">10893.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K26">
         <is>
-          <t xml:space="preserve">3113.00</t>
+          <t xml:space="preserve">3143.87</t>
         </is>
       </c>
     </row>
@@ -1362,39 +1362,39 @@
           <t xml:space="preserve">05:00 - 05:15</t>
         </is>
       </c>
-      <c s="9" t="inlineStr" r="D27">
-        <is>
-          <t xml:space="preserve">9478.80</t>
-        </is>
-      </c>
-      <c s="9" t="inlineStr" r="F27">
-        <is>
-          <t xml:space="preserve">12481.40</t>
-        </is>
-      </c>
-      <c s="9" t="inlineStr" r="G27">
-        <is>
-          <t xml:space="preserve">7572.80</t>
-        </is>
-      </c>
-      <c s="9" t="inlineStr" r="H27">
-        <is>
-          <t xml:space="preserve">7562.40</t>
-        </is>
-      </c>
-      <c s="9" t="inlineStr" r="I27">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c s="9" t="inlineStr" r="J27">
-        <is>
-          <t xml:space="preserve">7562.40</t>
+      <c s="14" t="inlineStr" r="D27">
+        <is>
+          <t xml:space="preserve">12324.00</t>
+        </is>
+      </c>
+      <c s="14" t="inlineStr" r="F27">
+        <is>
+          <t xml:space="preserve">14374.80</t>
+        </is>
+      </c>
+      <c s="14" t="inlineStr" r="G27">
+        <is>
+          <t xml:space="preserve">11026.70</t>
+        </is>
+      </c>
+      <c s="14" t="inlineStr" r="H27">
+        <is>
+          <t xml:space="preserve">10274.10</t>
+        </is>
+      </c>
+      <c s="14" t="inlineStr" r="I27">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c s="14" t="inlineStr" r="J27">
+        <is>
+          <t xml:space="preserve">10274.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K27">
         <is>
-          <t xml:space="preserve">3229.85</t>
+          <t xml:space="preserve">3299.83</t>
         </is>
       </c>
     </row>
@@ -1406,39 +1406,39 @@
           <t xml:space="preserve">05:15 - 05:30</t>
         </is>
       </c>
-      <c s="9" t="inlineStr" r="D28">
-        <is>
-          <t xml:space="preserve">9768.80</t>
-        </is>
-      </c>
-      <c s="9" t="inlineStr" r="F28">
-        <is>
-          <t xml:space="preserve">11888.40</t>
-        </is>
-      </c>
-      <c s="9" t="inlineStr" r="G28">
-        <is>
-          <t xml:space="preserve">7856.20</t>
-        </is>
-      </c>
-      <c s="9" t="inlineStr" r="H28">
-        <is>
-          <t xml:space="preserve">7845.80</t>
-        </is>
-      </c>
-      <c s="9" t="inlineStr" r="I28">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c s="9" t="inlineStr" r="J28">
-        <is>
-          <t xml:space="preserve">7845.80</t>
+      <c s="14" t="inlineStr" r="D28">
+        <is>
+          <t xml:space="preserve">12349.60</t>
+        </is>
+      </c>
+      <c s="14" t="inlineStr" r="F28">
+        <is>
+          <t xml:space="preserve">14199.70</t>
+        </is>
+      </c>
+      <c s="14" t="inlineStr" r="G28">
+        <is>
+          <t xml:space="preserve">11031.71</t>
+        </is>
+      </c>
+      <c s="14" t="inlineStr" r="H28">
+        <is>
+          <t xml:space="preserve">9949.50</t>
+        </is>
+      </c>
+      <c s="14" t="inlineStr" r="I28">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c s="14" t="inlineStr" r="J28">
+        <is>
+          <t xml:space="preserve">9949.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K28">
         <is>
-          <t xml:space="preserve">3294.86</t>
+          <t xml:space="preserve">3308.39</t>
         </is>
       </c>
     </row>
@@ -1452,22 +1452,22 @@
       </c>
       <c s="14" t="inlineStr" r="D29">
         <is>
-          <t xml:space="preserve">9855.30</t>
+          <t xml:space="preserve">12573.80</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="F29">
         <is>
-          <t xml:space="preserve">11256.30</t>
+          <t xml:space="preserve">14199.20</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="G29">
         <is>
-          <t xml:space="preserve">7897.90</t>
+          <t xml:space="preserve">11273.00</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="H29">
         <is>
-          <t xml:space="preserve">7606.31</t>
+          <t xml:space="preserve">10121.10</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="I29">
@@ -1477,12 +1477,12 @@
       </c>
       <c s="14" t="inlineStr" r="J29">
         <is>
-          <t xml:space="preserve">7606.31</t>
+          <t xml:space="preserve">10121.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K29">
         <is>
-          <t xml:space="preserve">3359.02</t>
+          <t xml:space="preserve">3299.20</t>
         </is>
       </c>
     </row>
@@ -1496,22 +1496,22 @@
       </c>
       <c s="14" t="inlineStr" r="D30">
         <is>
-          <t xml:space="preserve">10141.10</t>
+          <t xml:space="preserve">12882.00</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="F30">
         <is>
-          <t xml:space="preserve">11904.30</t>
+          <t xml:space="preserve">14258.80</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="G30">
         <is>
-          <t xml:space="preserve">8187.10</t>
+          <t xml:space="preserve">11557.70</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="H30">
         <is>
-          <t xml:space="preserve">7692.21</t>
+          <t xml:space="preserve">10371.40</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="I30">
@@ -1521,12 +1521,12 @@
       </c>
       <c s="14" t="inlineStr" r="J30">
         <is>
-          <t xml:space="preserve">7692.21</t>
+          <t xml:space="preserve">10371.40</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K30">
         <is>
-          <t xml:space="preserve">3308.11</t>
+          <t xml:space="preserve">3374.99</t>
         </is>
       </c>
     </row>
@@ -1542,22 +1542,22 @@
       </c>
       <c s="14" t="inlineStr" r="D31">
         <is>
-          <t xml:space="preserve">10077.30</t>
+          <t xml:space="preserve">13281.90</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="F31">
         <is>
-          <t xml:space="preserve">12020.10</t>
+          <t xml:space="preserve">13478.80</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="G31">
         <is>
-          <t xml:space="preserve">9338.50</t>
+          <t xml:space="preserve">12054.90</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="H31">
         <is>
-          <t xml:space="preserve">8164.10</t>
+          <t xml:space="preserve">10482.90</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="I31">
@@ -1567,12 +1567,12 @@
       </c>
       <c s="14" t="inlineStr" r="J31">
         <is>
-          <t xml:space="preserve">8164.10</t>
+          <t xml:space="preserve">10482.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K31">
         <is>
-          <t xml:space="preserve">3379.21</t>
+          <t xml:space="preserve">3920.31</t>
         </is>
       </c>
     </row>
@@ -1586,22 +1586,22 @@
       </c>
       <c s="14" t="inlineStr" r="D32">
         <is>
-          <t xml:space="preserve">10685.90</t>
+          <t xml:space="preserve">13762.80</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="F32">
         <is>
-          <t xml:space="preserve">11666.20</t>
+          <t xml:space="preserve">12952.90</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="G32">
         <is>
-          <t xml:space="preserve">9837.30</t>
+          <t xml:space="preserve">12027.80</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="H32">
         <is>
-          <t xml:space="preserve">8822.70</t>
+          <t xml:space="preserve">10694.73</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="I32">
@@ -1611,12 +1611,12 @@
       </c>
       <c s="14" t="inlineStr" r="J32">
         <is>
-          <t xml:space="preserve">8822.70</t>
+          <t xml:space="preserve">10694.73</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K32">
         <is>
-          <t xml:space="preserve">3552.05</t>
+          <t xml:space="preserve">4444.78</t>
         </is>
       </c>
     </row>
@@ -1630,22 +1630,22 @@
       </c>
       <c s="14" t="inlineStr" r="D33">
         <is>
-          <t xml:space="preserve">11066.00</t>
+          <t xml:space="preserve">14159.60</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="F33">
         <is>
-          <t xml:space="preserve">11105.10</t>
+          <t xml:space="preserve">13609.00</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="G33">
         <is>
-          <t xml:space="preserve">9678.28</t>
+          <t xml:space="preserve">12532.70</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="H33">
         <is>
-          <t xml:space="preserve">9076.60</t>
+          <t xml:space="preserve">10732.73</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="I33">
@@ -1655,12 +1655,12 @@
       </c>
       <c s="14" t="inlineStr" r="J33">
         <is>
-          <t xml:space="preserve">9076.60</t>
+          <t xml:space="preserve">10732.73</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K33">
         <is>
-          <t xml:space="preserve">4021.65</t>
+          <t xml:space="preserve">4382.05</t>
         </is>
       </c>
     </row>
@@ -1674,22 +1674,22 @@
       </c>
       <c s="14" t="inlineStr" r="D34">
         <is>
-          <t xml:space="preserve">11683.80</t>
+          <t xml:space="preserve">14312.80</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="F34">
         <is>
-          <t xml:space="preserve">11179.40</t>
+          <t xml:space="preserve">13843.50</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="G34">
         <is>
-          <t xml:space="preserve">10128.90</t>
+          <t xml:space="preserve">12718.20</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="H34">
         <is>
-          <t xml:space="preserve">9445.73</t>
+          <t xml:space="preserve">10505.83</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="I34">
@@ -1699,12 +1699,12 @@
       </c>
       <c s="14" t="inlineStr" r="J34">
         <is>
-          <t xml:space="preserve">9445.73</t>
+          <t xml:space="preserve">10505.83</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K34">
         <is>
-          <t xml:space="preserve">4400.65</t>
+          <t xml:space="preserve">4043.96</t>
         </is>
       </c>
     </row>
@@ -1720,22 +1720,22 @@
       </c>
       <c s="14" t="inlineStr" r="D35">
         <is>
-          <t xml:space="preserve">12150.20</t>
+          <t xml:space="preserve">14183.50</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="F35">
         <is>
-          <t xml:space="preserve">10955.00</t>
+          <t xml:space="preserve">13475.70</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="G35">
         <is>
-          <t xml:space="preserve">10107.80</t>
+          <t xml:space="preserve">12250.40</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="H35">
         <is>
-          <t xml:space="preserve">9337.40</t>
+          <t xml:space="preserve">10401.93</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="I35">
@@ -1745,12 +1745,12 @@
       </c>
       <c s="14" t="inlineStr" r="J35">
         <is>
-          <t xml:space="preserve">9337.40</t>
+          <t xml:space="preserve">10401.93</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K35">
         <is>
-          <t xml:space="preserve">4789.49</t>
+          <t xml:space="preserve">4250.85</t>
         </is>
       </c>
     </row>
@@ -1764,22 +1764,22 @@
       </c>
       <c s="14" t="inlineStr" r="D36">
         <is>
-          <t xml:space="preserve">13121.70</t>
+          <t xml:space="preserve">13904.60</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="F36">
         <is>
-          <t xml:space="preserve">11223.40</t>
+          <t xml:space="preserve">13430.00</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="G36">
         <is>
-          <t xml:space="preserve">10507.20</t>
+          <t xml:space="preserve">12123.10</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="H36">
         <is>
-          <t xml:space="preserve">10093.10</t>
+          <t xml:space="preserve">10424.03</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="I36">
@@ -1789,12 +1789,12 @@
       </c>
       <c s="14" t="inlineStr" r="J36">
         <is>
-          <t xml:space="preserve">10093.10</t>
+          <t xml:space="preserve">10424.03</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K36">
         <is>
-          <t xml:space="preserve">5250.75</t>
+          <t xml:space="preserve">4144.45</t>
         </is>
       </c>
     </row>
@@ -1808,22 +1808,22 @@
       </c>
       <c s="14" t="inlineStr" r="D37">
         <is>
-          <t xml:space="preserve">12970.70</t>
+          <t xml:space="preserve">13320.30</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="F37">
         <is>
-          <t xml:space="preserve">10646.90</t>
+          <t xml:space="preserve">13325.50</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="G37">
         <is>
-          <t xml:space="preserve">10084.90</t>
+          <t xml:space="preserve">11857.40</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="H37">
         <is>
-          <t xml:space="preserve">9927.53</t>
+          <t xml:space="preserve">10337.83</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="I37">
@@ -1833,12 +1833,12 @@
       </c>
       <c s="14" t="inlineStr" r="J37">
         <is>
-          <t xml:space="preserve">9927.53</t>
+          <t xml:space="preserve">10337.83</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K37">
         <is>
-          <t xml:space="preserve">6000.72</t>
+          <t xml:space="preserve">3900.57</t>
         </is>
       </c>
     </row>
@@ -1852,22 +1852,22 @@
       </c>
       <c s="14" t="inlineStr" r="D38">
         <is>
-          <t xml:space="preserve">12727.50</t>
+          <t xml:space="preserve">12795.60</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="F38">
         <is>
-          <t xml:space="preserve">10288.70</t>
+          <t xml:space="preserve">13264.70</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="G38">
         <is>
-          <t xml:space="preserve">9726.70</t>
+          <t xml:space="preserve">11638.60</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="H38">
         <is>
-          <t xml:space="preserve">9578.40</t>
+          <t xml:space="preserve">10329.60</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="I38">
@@ -1877,12 +1877,12 @@
       </c>
       <c s="14" t="inlineStr" r="J38">
         <is>
-          <t xml:space="preserve">9578.40</t>
+          <t xml:space="preserve">10329.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K38">
         <is>
-          <t xml:space="preserve">6666.77</t>
+          <t xml:space="preserve">3549.24</t>
         </is>
       </c>
     </row>
@@ -1898,22 +1898,22 @@
       </c>
       <c s="14" t="inlineStr" r="D39">
         <is>
-          <t xml:space="preserve">11948.80</t>
+          <t xml:space="preserve">11777.30</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="F39">
         <is>
-          <t xml:space="preserve">10956.70</t>
+          <t xml:space="preserve">13186.60</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="G39">
         <is>
-          <t xml:space="preserve">9967.50</t>
+          <t xml:space="preserve">10942.10</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="H39">
         <is>
-          <t xml:space="preserve">9324.60</t>
+          <t xml:space="preserve">9824.30</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="I39">
@@ -1923,12 +1923,12 @@
       </c>
       <c s="14" t="inlineStr" r="J39">
         <is>
-          <t xml:space="preserve">9324.60</t>
+          <t xml:space="preserve">9824.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K39">
         <is>
-          <t xml:space="preserve">4500.82</t>
+          <t xml:space="preserve">3398.42</t>
         </is>
       </c>
     </row>
@@ -1942,22 +1942,22 @@
       </c>
       <c s="14" t="inlineStr" r="D40">
         <is>
-          <t xml:space="preserve">11787.10</t>
+          <t xml:space="preserve">11351.60</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="F40">
         <is>
-          <t xml:space="preserve">10343.60</t>
+          <t xml:space="preserve">13326.90</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="G40">
         <is>
-          <t xml:space="preserve">9527.40</t>
+          <t xml:space="preserve">10630.10</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="H40">
         <is>
-          <t xml:space="preserve">9059.13</t>
+          <t xml:space="preserve">9922.80</t>
         </is>
       </c>
       <c s="14" t="inlineStr" r="I40">
@@ -1967,12 +1967,12 @@
       </c>
       <c s="14" t="inlineStr" r="J40">
         <is>
-          <t xml:space="preserve">9059.13</t>
+          <t xml:space="preserve">9922.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K40">
         <is>
-          <t xml:space="preserve">5250.35</t>
+          <t xml:space="preserve">3299.67</t>
         </is>
       </c>
     </row>
@@ -1986,22 +1986,22 @@
       </c>
       <c s="9" t="inlineStr" r="D41">
         <is>
-          <t xml:space="preserve">11385.50</t>
+          <t xml:space="preserve">11211.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F41">
         <is>
-          <t xml:space="preserve">9916.80</t>
+          <t xml:space="preserve">12748.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G41">
         <is>
-          <t xml:space="preserve">9130.60</t>
+          <t xml:space="preserve">10476.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H41">
         <is>
-          <t xml:space="preserve">8776.40</t>
+          <t xml:space="preserve">10216.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I41">
@@ -2011,12 +2011,12 @@
       </c>
       <c s="9" t="inlineStr" r="J41">
         <is>
-          <t xml:space="preserve">8776.40</t>
+          <t xml:space="preserve">10216.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K41">
         <is>
-          <t xml:space="preserve">5250.18</t>
+          <t xml:space="preserve">3398.79</t>
         </is>
       </c>
     </row>
@@ -2030,22 +2030,22 @@
       </c>
       <c s="9" t="inlineStr" r="D42">
         <is>
-          <t xml:space="preserve">10869.20</t>
+          <t xml:space="preserve">10986.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F42">
         <is>
-          <t xml:space="preserve">8903.50</t>
+          <t xml:space="preserve">12301.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G42">
         <is>
-          <t xml:space="preserve">8361.50</t>
+          <t xml:space="preserve">10231.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H42">
         <is>
-          <t xml:space="preserve">8109.10</t>
+          <t xml:space="preserve">10092.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I42">
@@ -2055,12 +2055,12 @@
       </c>
       <c s="9" t="inlineStr" r="J42">
         <is>
-          <t xml:space="preserve">8109.10</t>
+          <t xml:space="preserve">10092.00</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K42">
         <is>
-          <t xml:space="preserve">6000.36</t>
+          <t xml:space="preserve">3469.05</t>
         </is>
       </c>
     </row>
@@ -2076,22 +2076,22 @@
       </c>
       <c s="9" t="inlineStr" r="D43">
         <is>
-          <t xml:space="preserve">10490.50</t>
+          <t xml:space="preserve">10900.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F43">
         <is>
-          <t xml:space="preserve">9150.40</t>
+          <t xml:space="preserve">12153.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G43">
         <is>
-          <t xml:space="preserve">8259.40</t>
+          <t xml:space="preserve">9973.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H43">
         <is>
-          <t xml:space="preserve">8038.10</t>
+          <t xml:space="preserve">9912.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I43">
@@ -2101,12 +2101,12 @@
       </c>
       <c s="9" t="inlineStr" r="J43">
         <is>
-          <t xml:space="preserve">8038.10</t>
+          <t xml:space="preserve">9912.00</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K43">
         <is>
-          <t xml:space="preserve">4999.07</t>
+          <t xml:space="preserve">3398.13</t>
         </is>
       </c>
     </row>
@@ -2120,22 +2120,22 @@
       </c>
       <c s="9" t="inlineStr" r="D44">
         <is>
-          <t xml:space="preserve">10477.90</t>
+          <t xml:space="preserve">10881.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F44">
         <is>
-          <t xml:space="preserve">8538.50</t>
+          <t xml:space="preserve">11282.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G44">
         <is>
-          <t xml:space="preserve">7940.10</t>
+          <t xml:space="preserve">9686.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H44">
         <is>
-          <t xml:space="preserve">7750.00</t>
+          <t xml:space="preserve">9625.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I44">
@@ -2145,12 +2145,12 @@
       </c>
       <c s="9" t="inlineStr" r="J44">
         <is>
-          <t xml:space="preserve">7750.00</t>
+          <t xml:space="preserve">9625.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K44">
         <is>
-          <t xml:space="preserve">6000.32</t>
+          <t xml:space="preserve">3679.74</t>
         </is>
       </c>
     </row>
@@ -2164,22 +2164,22 @@
       </c>
       <c s="9" t="inlineStr" r="D45">
         <is>
-          <t xml:space="preserve">9874.70</t>
+          <t xml:space="preserve">11383.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F45">
         <is>
-          <t xml:space="preserve">8581.00</t>
+          <t xml:space="preserve">11041.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G45">
         <is>
-          <t xml:space="preserve">7645.00</t>
+          <t xml:space="preserve">9719.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H45">
         <is>
-          <t xml:space="preserve">7651.80</t>
+          <t xml:space="preserve">9651.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I45">
@@ -2189,12 +2189,12 @@
       </c>
       <c s="9" t="inlineStr" r="J45">
         <is>
-          <t xml:space="preserve">7651.80</t>
+          <t xml:space="preserve">9651.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K45">
         <is>
-          <t xml:space="preserve">4999.10</t>
+          <t xml:space="preserve">4144.97</t>
         </is>
       </c>
     </row>
@@ -2208,22 +2208,22 @@
       </c>
       <c s="9" t="inlineStr" r="D46">
         <is>
-          <t xml:space="preserve">9622.80</t>
+          <t xml:space="preserve">11267.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F46">
         <is>
-          <t xml:space="preserve">8640.10</t>
+          <t xml:space="preserve">10588.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G46">
         <is>
-          <t xml:space="preserve">7424.90</t>
+          <t xml:space="preserve">9435.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H46">
         <is>
-          <t xml:space="preserve">7431.70</t>
+          <t xml:space="preserve">9363.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I46">
@@ -2233,12 +2233,12 @@
       </c>
       <c s="9" t="inlineStr" r="J46">
         <is>
-          <t xml:space="preserve">7431.70</t>
+          <t xml:space="preserve">9363.00</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K46">
         <is>
-          <t xml:space="preserve">4362.55</t>
+          <t xml:space="preserve">4400.97</t>
         </is>
       </c>
     </row>
@@ -2254,22 +2254,22 @@
       </c>
       <c s="9" t="inlineStr" r="D47">
         <is>
-          <t xml:space="preserve">9180.10</t>
+          <t xml:space="preserve">11394.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F47">
         <is>
-          <t xml:space="preserve">8478.40</t>
+          <t xml:space="preserve">11631.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G47">
         <is>
-          <t xml:space="preserve">7065.95</t>
+          <t xml:space="preserve">9744.33</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H47">
         <is>
-          <t xml:space="preserve">7065.95</t>
+          <t xml:space="preserve">9677.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I47">
@@ -2279,12 +2279,12 @@
       </c>
       <c s="9" t="inlineStr" r="J47">
         <is>
-          <t xml:space="preserve">7065.95</t>
+          <t xml:space="preserve">9677.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K47">
         <is>
-          <t xml:space="preserve">4201.75</t>
+          <t xml:space="preserve">3999.44</t>
         </is>
       </c>
     </row>
@@ -2298,22 +2298,22 @@
       </c>
       <c s="9" t="inlineStr" r="D48">
         <is>
-          <t xml:space="preserve">9107.80</t>
+          <t xml:space="preserve">11309.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F48">
         <is>
-          <t xml:space="preserve">8256.30</t>
+          <t xml:space="preserve">11732.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G48">
         <is>
-          <t xml:space="preserve">6873.50</t>
+          <t xml:space="preserve">9808.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H48">
         <is>
-          <t xml:space="preserve">6873.50</t>
+          <t xml:space="preserve">9717.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I48">
@@ -2323,12 +2323,12 @@
       </c>
       <c s="9" t="inlineStr" r="J48">
         <is>
-          <t xml:space="preserve">6873.50</t>
+          <t xml:space="preserve">9717.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K48">
         <is>
-          <t xml:space="preserve">4362.06</t>
+          <t xml:space="preserve">3680.52</t>
         </is>
       </c>
     </row>
@@ -2342,22 +2342,22 @@
       </c>
       <c s="9" t="inlineStr" r="D49">
         <is>
-          <t xml:space="preserve">8824.30</t>
+          <t xml:space="preserve">11578.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F49">
         <is>
-          <t xml:space="preserve">8089.60</t>
+          <t xml:space="preserve">11645.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G49">
         <is>
-          <t xml:space="preserve">6554.70</t>
+          <t xml:space="preserve">9802.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H49">
         <is>
-          <t xml:space="preserve">6554.70</t>
+          <t xml:space="preserve">9768.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I49">
@@ -2367,12 +2367,12 @@
       </c>
       <c s="9" t="inlineStr" r="J49">
         <is>
-          <t xml:space="preserve">6554.70</t>
+          <t xml:space="preserve">9768.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K49">
         <is>
-          <t xml:space="preserve">4012.10</t>
+          <t xml:space="preserve">4100.90</t>
         </is>
       </c>
     </row>
@@ -2386,22 +2386,22 @@
       </c>
       <c s="9" t="inlineStr" r="D50">
         <is>
-          <t xml:space="preserve">8355.50</t>
+          <t xml:space="preserve">11664.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F50">
         <is>
-          <t xml:space="preserve">8144.20</t>
+          <t xml:space="preserve">11824.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G50">
         <is>
-          <t xml:space="preserve">6415.75</t>
+          <t xml:space="preserve">9911.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H50">
         <is>
-          <t xml:space="preserve">6415.75</t>
+          <t xml:space="preserve">9835.51</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I50">
@@ -2411,12 +2411,12 @@
       </c>
       <c s="9" t="inlineStr" r="J50">
         <is>
-          <t xml:space="preserve">6415.75</t>
+          <t xml:space="preserve">9835.51</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K50">
         <is>
-          <t xml:space="preserve">3600.09</t>
+          <t xml:space="preserve">3857.52</t>
         </is>
       </c>
     </row>
@@ -2432,22 +2432,22 @@
       </c>
       <c s="9" t="inlineStr" r="D51">
         <is>
-          <t xml:space="preserve">8514.40</t>
+          <t xml:space="preserve">11883.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F51">
         <is>
-          <t xml:space="preserve">8003.90</t>
+          <t xml:space="preserve">11847.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G51">
         <is>
-          <t xml:space="preserve">6602.85</t>
+          <t xml:space="preserve">9999.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H51">
         <is>
-          <t xml:space="preserve">6637.30</t>
+          <t xml:space="preserve">9905.88</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I51">
@@ -2457,12 +2457,12 @@
       </c>
       <c s="9" t="inlineStr" r="J51">
         <is>
-          <t xml:space="preserve">6637.30</t>
+          <t xml:space="preserve">9905.88</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K51">
         <is>
-          <t xml:space="preserve">4010.95</t>
+          <t xml:space="preserve">3812.40</t>
         </is>
       </c>
     </row>
@@ -2476,22 +2476,22 @@
       </c>
       <c s="9" t="inlineStr" r="D52">
         <is>
-          <t xml:space="preserve">8487.30</t>
+          <t xml:space="preserve">12004.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F52">
         <is>
-          <t xml:space="preserve">8083.10</t>
+          <t xml:space="preserve">12186.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G52">
         <is>
-          <t xml:space="preserve">6631.55</t>
+          <t xml:space="preserve">10304.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H52">
         <is>
-          <t xml:space="preserve">6650.50</t>
+          <t xml:space="preserve">10201.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I52">
@@ -2501,12 +2501,12 @@
       </c>
       <c s="9" t="inlineStr" r="J52">
         <is>
-          <t xml:space="preserve">6650.50</t>
+          <t xml:space="preserve">10201.40</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K52">
         <is>
-          <t xml:space="preserve">4000.95</t>
+          <t xml:space="preserve">3640.65</t>
         </is>
       </c>
     </row>
@@ -2520,22 +2520,22 @@
       </c>
       <c s="9" t="inlineStr" r="D53">
         <is>
-          <t xml:space="preserve">8057.20</t>
+          <t xml:space="preserve">12223.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F53">
         <is>
-          <t xml:space="preserve">8223.10</t>
+          <t xml:space="preserve">12440.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G53">
         <is>
-          <t xml:space="preserve">6294.80</t>
+          <t xml:space="preserve">10515.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H53">
         <is>
-          <t xml:space="preserve">6520.40</t>
+          <t xml:space="preserve">10412.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I53">
@@ -2545,12 +2545,12 @@
       </c>
       <c s="9" t="inlineStr" r="J53">
         <is>
-          <t xml:space="preserve">6520.40</t>
+          <t xml:space="preserve">10412.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K53">
         <is>
-          <t xml:space="preserve">3769.13</t>
+          <t xml:space="preserve">3650.67</t>
         </is>
       </c>
     </row>
@@ -2564,22 +2564,22 @@
       </c>
       <c s="9" t="inlineStr" r="D54">
         <is>
-          <t xml:space="preserve">7930.30</t>
+          <t xml:space="preserve">11943.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F54">
         <is>
-          <t xml:space="preserve">8797.80</t>
+          <t xml:space="preserve">12709.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G54">
         <is>
-          <t xml:space="preserve">6520.20</t>
+          <t xml:space="preserve">10320.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H54">
         <is>
-          <t xml:space="preserve">6570.20</t>
+          <t xml:space="preserve">10282.41</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I54">
@@ -2589,12 +2589,12 @@
       </c>
       <c s="9" t="inlineStr" r="J54">
         <is>
-          <t xml:space="preserve">6570.20</t>
+          <t xml:space="preserve">10282.41</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K54">
         <is>
-          <t xml:space="preserve">3408.84</t>
+          <t xml:space="preserve">3374.61</t>
         </is>
       </c>
     </row>
@@ -2610,22 +2610,22 @@
       </c>
       <c s="9" t="inlineStr" r="D55">
         <is>
-          <t xml:space="preserve">7824.20</t>
+          <t xml:space="preserve">11567.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F55">
         <is>
-          <t xml:space="preserve">8968.50</t>
+          <t xml:space="preserve">12595.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G55">
         <is>
-          <t xml:space="preserve">6499.80</t>
+          <t xml:space="preserve">10127.38</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H55">
         <is>
-          <t xml:space="preserve">6536.00</t>
+          <t xml:space="preserve">10117.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I55">
@@ -2635,12 +2635,12 @@
       </c>
       <c s="9" t="inlineStr" r="J55">
         <is>
-          <t xml:space="preserve">6536.00</t>
+          <t xml:space="preserve">10117.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K55">
         <is>
-          <t xml:space="preserve">3305.10</t>
+          <t xml:space="preserve">3308.84</t>
         </is>
       </c>
     </row>
@@ -2654,22 +2654,22 @@
       </c>
       <c s="9" t="inlineStr" r="D56">
         <is>
-          <t xml:space="preserve">7783.50</t>
+          <t xml:space="preserve">11527.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F56">
         <is>
-          <t xml:space="preserve">9027.40</t>
+          <t xml:space="preserve">12428.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G56">
         <is>
-          <t xml:space="preserve">6492.30</t>
+          <t xml:space="preserve">10171.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H56">
         <is>
-          <t xml:space="preserve">6498.50</t>
+          <t xml:space="preserve">10162.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I56">
@@ -2679,12 +2679,12 @@
       </c>
       <c s="9" t="inlineStr" r="J56">
         <is>
-          <t xml:space="preserve">6498.50</t>
+          <t xml:space="preserve">10162.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K56">
         <is>
-          <t xml:space="preserve">3294.39</t>
+          <t xml:space="preserve">3469.56</t>
         </is>
       </c>
     </row>
@@ -2698,22 +2698,22 @@
       </c>
       <c s="9" t="inlineStr" r="D57">
         <is>
-          <t xml:space="preserve">7771.50</t>
+          <t xml:space="preserve">11626.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F57">
         <is>
-          <t xml:space="preserve">9146.80</t>
+          <t xml:space="preserve">13117.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G57">
         <is>
-          <t xml:space="preserve">6552.20</t>
+          <t xml:space="preserve">10290.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H57">
         <is>
-          <t xml:space="preserve">6554.80</t>
+          <t xml:space="preserve">10290.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I57">
@@ -2723,12 +2723,12 @@
       </c>
       <c s="9" t="inlineStr" r="J57">
         <is>
-          <t xml:space="preserve">6554.80</t>
+          <t xml:space="preserve">10290.00</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K57">
         <is>
-          <t xml:space="preserve">3113.85</t>
+          <t xml:space="preserve">3300.71</t>
         </is>
       </c>
     </row>
@@ -2742,22 +2742,22 @@
       </c>
       <c s="9" t="inlineStr" r="D58">
         <is>
-          <t xml:space="preserve">7995.10</t>
+          <t xml:space="preserve">11322.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F58">
         <is>
-          <t xml:space="preserve">9724.20</t>
+          <t xml:space="preserve">13540.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G58">
         <is>
-          <t xml:space="preserve">6876.00</t>
+          <t xml:space="preserve">10138.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H58">
         <is>
-          <t xml:space="preserve">6955.20</t>
+          <t xml:space="preserve">10128.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I58">
@@ -2767,12 +2767,12 @@
       </c>
       <c s="9" t="inlineStr" r="J58">
         <is>
-          <t xml:space="preserve">6955.20</t>
+          <t xml:space="preserve">10128.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K58">
         <is>
-          <t xml:space="preserve">3113.30</t>
+          <t xml:space="preserve">3199.12</t>
         </is>
       </c>
     </row>
@@ -2788,22 +2788,22 @@
       </c>
       <c s="9" t="inlineStr" r="D59">
         <is>
-          <t xml:space="preserve">8458.80</t>
+          <t xml:space="preserve">11051.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F59">
         <is>
-          <t xml:space="preserve">10757.60</t>
+          <t xml:space="preserve">14503.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G59">
         <is>
-          <t xml:space="preserve">7455.30</t>
+          <t xml:space="preserve">10023.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H59">
         <is>
-          <t xml:space="preserve">7506.80</t>
+          <t xml:space="preserve">10014.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I59">
@@ -2813,12 +2813,12 @@
       </c>
       <c s="9" t="inlineStr" r="J59">
         <is>
-          <t xml:space="preserve">7506.80</t>
+          <t xml:space="preserve">10014.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K59">
         <is>
-          <t xml:space="preserve">3098.76</t>
+          <t xml:space="preserve">3059.84</t>
         </is>
       </c>
     </row>
@@ -2832,22 +2832,22 @@
       </c>
       <c s="9" t="inlineStr" r="D60">
         <is>
-          <t xml:space="preserve">8674.10</t>
+          <t xml:space="preserve">11058.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F60">
         <is>
-          <t xml:space="preserve">11515.20</t>
+          <t xml:space="preserve">15011.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G60">
         <is>
-          <t xml:space="preserve">7946.30</t>
+          <t xml:space="preserve">10031.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H60">
         <is>
-          <t xml:space="preserve">7961.70</t>
+          <t xml:space="preserve">10028.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I60">
@@ -2857,12 +2857,12 @@
       </c>
       <c s="9" t="inlineStr" r="J60">
         <is>
-          <t xml:space="preserve">7961.70</t>
+          <t xml:space="preserve">10028.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K60">
         <is>
-          <t xml:space="preserve">2947.79</t>
+          <t xml:space="preserve">3051.18</t>
         </is>
       </c>
     </row>
@@ -2876,22 +2876,22 @@
       </c>
       <c s="9" t="inlineStr" r="D61">
         <is>
-          <t xml:space="preserve">8778.60</t>
+          <t xml:space="preserve">11220.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F61">
         <is>
-          <t xml:space="preserve">12194.70</t>
+          <t xml:space="preserve">15415.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G61">
         <is>
-          <t xml:space="preserve">8106.30</t>
+          <t xml:space="preserve">10263.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H61">
         <is>
-          <t xml:space="preserve">8111.80</t>
+          <t xml:space="preserve">10253.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I61">
@@ -2901,12 +2901,12 @@
       </c>
       <c s="9" t="inlineStr" r="J61">
         <is>
-          <t xml:space="preserve">8111.80</t>
+          <t xml:space="preserve">10253.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K61">
         <is>
-          <t xml:space="preserve">2899.86</t>
+          <t xml:space="preserve">2990.53</t>
         </is>
       </c>
     </row>
@@ -2920,22 +2920,22 @@
       </c>
       <c s="9" t="inlineStr" r="D62">
         <is>
-          <t xml:space="preserve">8716.80</t>
+          <t xml:space="preserve">11495.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F62">
         <is>
-          <t xml:space="preserve">12813.40</t>
+          <t xml:space="preserve">15913.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G62">
         <is>
-          <t xml:space="preserve">8088.90</t>
+          <t xml:space="preserve">10538.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H62">
         <is>
-          <t xml:space="preserve">8112.00</t>
+          <t xml:space="preserve">10528.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I62">
@@ -2945,12 +2945,12 @@
       </c>
       <c s="9" t="inlineStr" r="J62">
         <is>
-          <t xml:space="preserve">8112.00</t>
+          <t xml:space="preserve">10528.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K62">
         <is>
-          <t xml:space="preserve">2799.71</t>
+          <t xml:space="preserve">2979.75</t>
         </is>
       </c>
     </row>
@@ -2966,22 +2966,22 @@
       </c>
       <c s="9" t="inlineStr" r="D63">
         <is>
-          <t xml:space="preserve">9313.10</t>
+          <t xml:space="preserve">11914.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F63">
         <is>
-          <t xml:space="preserve">12914.60</t>
+          <t xml:space="preserve">15771.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G63">
         <is>
-          <t xml:space="preserve">8690.00</t>
+          <t xml:space="preserve">10918.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H63">
         <is>
-          <t xml:space="preserve">8688.40</t>
+          <t xml:space="preserve">10909.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I63">
@@ -2991,12 +2991,12 @@
       </c>
       <c s="9" t="inlineStr" r="J63">
         <is>
-          <t xml:space="preserve">8688.40</t>
+          <t xml:space="preserve">10909.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K63">
         <is>
-          <t xml:space="preserve">2883.93</t>
+          <t xml:space="preserve">2999.23</t>
         </is>
       </c>
     </row>
@@ -3010,22 +3010,22 @@
       </c>
       <c s="9" t="inlineStr" r="D64">
         <is>
-          <t xml:space="preserve">9743.20</t>
+          <t xml:space="preserve">12544.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F64">
         <is>
-          <t xml:space="preserve">13372.30</t>
+          <t xml:space="preserve">15625.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G64">
         <is>
-          <t xml:space="preserve">9037.10</t>
+          <t xml:space="preserve">11439.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H64">
         <is>
-          <t xml:space="preserve">9035.50</t>
+          <t xml:space="preserve">11430.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I64">
@@ -3035,12 +3035,12 @@
       </c>
       <c s="9" t="inlineStr" r="J64">
         <is>
-          <t xml:space="preserve">9035.50</t>
+          <t xml:space="preserve">11430.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K64">
         <is>
-          <t xml:space="preserve">2849.81</t>
+          <t xml:space="preserve">3059.88</t>
         </is>
       </c>
     </row>
@@ -3054,22 +3054,22 @@
       </c>
       <c s="9" t="inlineStr" r="D65">
         <is>
-          <t xml:space="preserve">10426.30</t>
+          <t xml:space="preserve">13073.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F65">
         <is>
-          <t xml:space="preserve">12996.90</t>
+          <t xml:space="preserve">15481.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G65">
         <is>
-          <t xml:space="preserve">9512.30</t>
+          <t xml:space="preserve">11971.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H65">
         <is>
-          <t xml:space="preserve">9647.50</t>
+          <t xml:space="preserve">11971.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I65">
@@ -3079,12 +3079,12 @@
       </c>
       <c s="9" t="inlineStr" r="J65">
         <is>
-          <t xml:space="preserve">9647.50</t>
+          <t xml:space="preserve">11971.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K65">
         <is>
-          <t xml:space="preserve">2953.99</t>
+          <t xml:space="preserve">3100.96</t>
         </is>
       </c>
     </row>
@@ -3098,22 +3098,22 @@
       </c>
       <c s="9" t="inlineStr" r="D66">
         <is>
-          <t xml:space="preserve">11152.00</t>
+          <t xml:space="preserve">13607.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F66">
         <is>
-          <t xml:space="preserve">12843.40</t>
+          <t xml:space="preserve">15104.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G66">
         <is>
-          <t xml:space="preserve">9993.50</t>
+          <t xml:space="preserve">12316.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H66">
         <is>
-          <t xml:space="preserve">10134.80</t>
+          <t xml:space="preserve">12307.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I66">
@@ -3123,12 +3123,12 @@
       </c>
       <c s="9" t="inlineStr" r="J66">
         <is>
-          <t xml:space="preserve">10134.80</t>
+          <t xml:space="preserve">12307.00</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K66">
         <is>
-          <t xml:space="preserve">3079.74</t>
+          <t xml:space="preserve">3279.92</t>
         </is>
       </c>
     </row>
@@ -3144,22 +3144,22 @@
       </c>
       <c s="9" t="inlineStr" r="D67">
         <is>
-          <t xml:space="preserve">11239.70</t>
+          <t xml:space="preserve">13942.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F67">
         <is>
-          <t xml:space="preserve">12467.90</t>
+          <t xml:space="preserve">14710.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G67">
         <is>
-          <t xml:space="preserve">9842.90</t>
+          <t xml:space="preserve">12385.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H67">
         <is>
-          <t xml:space="preserve">10021.90</t>
+          <t xml:space="preserve">12375.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I67">
@@ -3169,12 +3169,12 @@
       </c>
       <c s="9" t="inlineStr" r="J67">
         <is>
-          <t xml:space="preserve">10021.90</t>
+          <t xml:space="preserve">12375.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K67">
         <is>
-          <t xml:space="preserve">3100.33</t>
+          <t xml:space="preserve">3469.47</t>
         </is>
       </c>
     </row>
@@ -3188,22 +3188,22 @@
       </c>
       <c s="9" t="inlineStr" r="D68">
         <is>
-          <t xml:space="preserve">11744.60</t>
+          <t xml:space="preserve">14122.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F68">
         <is>
-          <t xml:space="preserve">12399.40</t>
+          <t xml:space="preserve">14571.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G68">
         <is>
-          <t xml:space="preserve">10067.40</t>
+          <t xml:space="preserve">12455.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H68">
         <is>
-          <t xml:space="preserve">10233.10</t>
+          <t xml:space="preserve">12448.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I68">
@@ -3213,12 +3213,12 @@
       </c>
       <c s="9" t="inlineStr" r="J68">
         <is>
-          <t xml:space="preserve">10233.10</t>
+          <t xml:space="preserve">12448.00</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K68">
         <is>
-          <t xml:space="preserve">3200.68</t>
+          <t xml:space="preserve">3559.75</t>
         </is>
       </c>
     </row>
@@ -3232,22 +3232,22 @@
       </c>
       <c s="9" t="inlineStr" r="D69">
         <is>
-          <t xml:space="preserve">12285.30</t>
+          <t xml:space="preserve">14050.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F69">
         <is>
-          <t xml:space="preserve">12297.40</t>
+          <t xml:space="preserve">14403.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G69">
         <is>
-          <t xml:space="preserve">10516.20</t>
+          <t xml:space="preserve">12358.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H69">
         <is>
-          <t xml:space="preserve">10621.20</t>
+          <t xml:space="preserve">12358.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I69">
@@ -3257,12 +3257,12 @@
       </c>
       <c s="9" t="inlineStr" r="J69">
         <is>
-          <t xml:space="preserve">10621.20</t>
+          <t xml:space="preserve">12358.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K69">
         <is>
-          <t xml:space="preserve">3429.30</t>
+          <t xml:space="preserve">3650.53</t>
         </is>
       </c>
     </row>
@@ -3274,39 +3274,39 @@
           <t xml:space="preserve">15:45 - 16:00</t>
         </is>
       </c>
-      <c s="14" t="inlineStr" r="D70">
-        <is>
-          <t xml:space="preserve">12693.30</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="F70">
-        <is>
-          <t xml:space="preserve">12271.20</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="G70">
-        <is>
-          <t xml:space="preserve">10846.80</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="H70">
-        <is>
-          <t xml:space="preserve">10690.30</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="I70">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="J70">
-        <is>
-          <t xml:space="preserve">10690.30</t>
+      <c s="9" t="inlineStr" r="D70">
+        <is>
+          <t xml:space="preserve">14401.80</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="F70">
+        <is>
+          <t xml:space="preserve">14331.70</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="G70">
+        <is>
+          <t xml:space="preserve">12334.80</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="H70">
+        <is>
+          <t xml:space="preserve">12329.50</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="I70">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="J70">
+        <is>
+          <t xml:space="preserve">12329.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K70">
         <is>
-          <t xml:space="preserve">3500.67</t>
+          <t xml:space="preserve">3699.53</t>
         </is>
       </c>
     </row>
@@ -3320,39 +3320,39 @@
           <t xml:space="preserve">16:00 - 16:15</t>
         </is>
       </c>
-      <c s="14" t="inlineStr" r="D71">
-        <is>
-          <t xml:space="preserve">13094.40</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="F71">
-        <is>
-          <t xml:space="preserve">12264.10</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="G71">
-        <is>
-          <t xml:space="preserve">10989.50</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="H71">
-        <is>
-          <t xml:space="preserve">10816.80</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="I71">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="J71">
-        <is>
-          <t xml:space="preserve">10816.80</t>
+      <c s="9" t="inlineStr" r="D71">
+        <is>
+          <t xml:space="preserve">13948.80</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="F71">
+        <is>
+          <t xml:space="preserve">14057.60</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="G71">
+        <is>
+          <t xml:space="preserve">12364.30</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="H71">
+        <is>
+          <t xml:space="preserve">12354.70</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="I71">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="J71">
+        <is>
+          <t xml:space="preserve">12354.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K71">
         <is>
-          <t xml:space="preserve">3650.85</t>
+          <t xml:space="preserve">3659.48</t>
         </is>
       </c>
     </row>
@@ -3364,39 +3364,39 @@
           <t xml:space="preserve">16:15 - 16:30</t>
         </is>
       </c>
-      <c s="14" t="inlineStr" r="D72">
-        <is>
-          <t xml:space="preserve">13303.90</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="F72">
-        <is>
-          <t xml:space="preserve">12191.40</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="G72">
-        <is>
-          <t xml:space="preserve">10939.90</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="H72">
-        <is>
-          <t xml:space="preserve">11066.78</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="I72">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="J72">
-        <is>
-          <t xml:space="preserve">11066.78</t>
+      <c s="9" t="inlineStr" r="D72">
+        <is>
+          <t xml:space="preserve">14599.50</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="F72">
+        <is>
+          <t xml:space="preserve">14106.80</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="G72">
+        <is>
+          <t xml:space="preserve">12740.30</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="H72">
+        <is>
+          <t xml:space="preserve">12730.70</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="I72">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="J72">
+        <is>
+          <t xml:space="preserve">12730.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K72">
         <is>
-          <t xml:space="preserve">3822.69</t>
+          <t xml:space="preserve">4144.19</t>
         </is>
       </c>
     </row>
@@ -3408,39 +3408,39 @@
           <t xml:space="preserve">16:30 - 16:45</t>
         </is>
       </c>
-      <c s="14" t="inlineStr" r="D73">
-        <is>
-          <t xml:space="preserve">13214.50</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="F73">
-        <is>
-          <t xml:space="preserve">12118.70</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="G73">
-        <is>
-          <t xml:space="preserve">11029.50</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="H73">
-        <is>
-          <t xml:space="preserve">11003.06</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="I73">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c s="14" t="inlineStr" r="J73">
-        <is>
-          <t xml:space="preserve">11003.06</t>
+      <c s="9" t="inlineStr" r="D73">
+        <is>
+          <t xml:space="preserve">15146.20</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="F73">
+        <is>
+          <t xml:space="preserve">14119.60</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="G73">
+        <is>
+          <t xml:space="preserve">13241.50</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="H73">
+        <is>
+          <t xml:space="preserve">13231.90</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="I73">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c s="9" t="inlineStr" r="J73">
+        <is>
+          <t xml:space="preserve">13231.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K73">
         <is>
-          <t xml:space="preserve">4362.12</t>
+          <t xml:space="preserve">4382.64</t>
         </is>
       </c>
     </row>
@@ -3454,22 +3454,22 @@
       </c>
       <c s="9" t="inlineStr" r="D74">
         <is>
-          <t xml:space="preserve">12877.90</t>
+          <t xml:space="preserve">15376.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F74">
         <is>
-          <t xml:space="preserve">11593.10</t>
+          <t xml:space="preserve">14259.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G74">
         <is>
-          <t xml:space="preserve">10674.80</t>
+          <t xml:space="preserve">13471.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H74">
         <is>
-          <t xml:space="preserve">10578.40</t>
+          <t xml:space="preserve">13462.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I74">
@@ -3479,12 +3479,12 @@
       </c>
       <c s="9" t="inlineStr" r="J74">
         <is>
-          <t xml:space="preserve">10578.40</t>
+          <t xml:space="preserve">13462.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K74">
         <is>
-          <t xml:space="preserve">4362.83</t>
+          <t xml:space="preserve">4382.82</t>
         </is>
       </c>
     </row>
@@ -3500,22 +3500,22 @@
       </c>
       <c s="9" t="inlineStr" r="D75">
         <is>
-          <t xml:space="preserve">12160.10</t>
+          <t xml:space="preserve">13908.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F75">
         <is>
-          <t xml:space="preserve">11549.50</t>
+          <t xml:space="preserve">14564.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G75">
         <is>
-          <t xml:space="preserve">10253.30</t>
+          <t xml:space="preserve">12691.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H75">
         <is>
-          <t xml:space="preserve">10475.10</t>
+          <t xml:space="preserve">12691.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I75">
@@ -3525,12 +3525,12 @@
       </c>
       <c s="9" t="inlineStr" r="J75">
         <is>
-          <t xml:space="preserve">10475.10</t>
+          <t xml:space="preserve">12691.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K75">
         <is>
-          <t xml:space="preserve">3779.63</t>
+          <t xml:space="preserve">3600.33</t>
         </is>
       </c>
     </row>
@@ -3544,22 +3544,22 @@
       </c>
       <c s="9" t="inlineStr" r="D76">
         <is>
-          <t xml:space="preserve">11930.20</t>
+          <t xml:space="preserve">13376.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F76">
         <is>
-          <t xml:space="preserve">10978.80</t>
+          <t xml:space="preserve">14482.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G76">
         <is>
-          <t xml:space="preserve">9723.13</t>
+          <t xml:space="preserve">12278.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H76">
         <is>
-          <t xml:space="preserve">9904.40</t>
+          <t xml:space="preserve">12268.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I76">
@@ -3569,12 +3569,12 @@
       </c>
       <c s="9" t="inlineStr" r="J76">
         <is>
-          <t xml:space="preserve">9904.40</t>
+          <t xml:space="preserve">12268.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K76">
         <is>
-          <t xml:space="preserve">4000.58</t>
+          <t xml:space="preserve">3442.50</t>
         </is>
       </c>
     </row>
@@ -3588,22 +3588,22 @@
       </c>
       <c s="9" t="inlineStr" r="D77">
         <is>
-          <t xml:space="preserve">11734.50</t>
+          <t xml:space="preserve">13155.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F77">
         <is>
-          <t xml:space="preserve">10404.10</t>
+          <t xml:space="preserve">14124.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G77">
         <is>
-          <t xml:space="preserve">9452.40</t>
+          <t xml:space="preserve">12078.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H77">
         <is>
-          <t xml:space="preserve">9527.80</t>
+          <t xml:space="preserve">12069.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I77">
@@ -3613,12 +3613,12 @@
       </c>
       <c s="9" t="inlineStr" r="J77">
         <is>
-          <t xml:space="preserve">9527.80</t>
+          <t xml:space="preserve">12069.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K77">
         <is>
-          <t xml:space="preserve">4362.41</t>
+          <t xml:space="preserve">3299.12</t>
         </is>
       </c>
     </row>
@@ -3632,22 +3632,22 @@
       </c>
       <c s="9" t="inlineStr" r="D78">
         <is>
-          <t xml:space="preserve">12073.70</t>
+          <t xml:space="preserve">12810.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F78">
         <is>
-          <t xml:space="preserve">9360.00</t>
+          <t xml:space="preserve">13677.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G78">
         <is>
-          <t xml:space="preserve">8816.80</t>
+          <t xml:space="preserve">11725.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H78">
         <is>
-          <t xml:space="preserve">9038.60</t>
+          <t xml:space="preserve">11715.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I78">
@@ -3657,12 +3657,12 @@
       </c>
       <c s="9" t="inlineStr" r="J78">
         <is>
-          <t xml:space="preserve">9038.60</t>
+          <t xml:space="preserve">11715.40</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K78">
         <is>
-          <t xml:space="preserve">6000.90</t>
+          <t xml:space="preserve">3374.53</t>
         </is>
       </c>
     </row>
@@ -3678,22 +3678,22 @@
       </c>
       <c s="9" t="inlineStr" r="D79">
         <is>
-          <t xml:space="preserve">10698.00</t>
+          <t xml:space="preserve">11910.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F79">
         <is>
-          <t xml:space="preserve">8812.20</t>
+          <t xml:space="preserve">13264.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G79">
         <is>
-          <t xml:space="preserve">8071.00</t>
+          <t xml:space="preserve">11055.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H79">
         <is>
-          <t xml:space="preserve">8321.00</t>
+          <t xml:space="preserve">11046.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I79">
@@ -3703,12 +3703,12 @@
       </c>
       <c s="9" t="inlineStr" r="J79">
         <is>
-          <t xml:space="preserve">8321.00</t>
+          <t xml:space="preserve">11046.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K79">
         <is>
-          <t xml:space="preserve">5250.99</t>
+          <t xml:space="preserve">3279.90</t>
         </is>
       </c>
     </row>
@@ -3722,22 +3722,22 @@
       </c>
       <c s="9" t="inlineStr" r="D80">
         <is>
-          <t xml:space="preserve">10568.00</t>
+          <t xml:space="preserve">12436.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F80">
         <is>
-          <t xml:space="preserve">8436.80</t>
+          <t xml:space="preserve">12053.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G80">
         <is>
-          <t xml:space="preserve">7676.80</t>
+          <t xml:space="preserve">11003.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H80">
         <is>
-          <t xml:space="preserve">7785.60</t>
+          <t xml:space="preserve">10993.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I80">
@@ -3747,12 +3747,12 @@
       </c>
       <c s="9" t="inlineStr" r="J80">
         <is>
-          <t xml:space="preserve">7785.60</t>
+          <t xml:space="preserve">10993.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K80">
         <is>
-          <t xml:space="preserve">5729.57</t>
+          <t xml:space="preserve">4529.48</t>
         </is>
       </c>
     </row>
@@ -3766,22 +3766,22 @@
       </c>
       <c s="9" t="inlineStr" r="D81">
         <is>
-          <t xml:space="preserve">11088.10</t>
+          <t xml:space="preserve">13000.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F81">
         <is>
-          <t xml:space="preserve">8192.80</t>
+          <t xml:space="preserve">11763.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G81">
         <is>
-          <t xml:space="preserve">7685.80</t>
+          <t xml:space="preserve">11061.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H81">
         <is>
-          <t xml:space="preserve">7805.80</t>
+          <t xml:space="preserve">11051.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I81">
@@ -3791,12 +3791,12 @@
       </c>
       <c s="9" t="inlineStr" r="J81">
         <is>
-          <t xml:space="preserve">7805.80</t>
+          <t xml:space="preserve">11051.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K81">
         <is>
-          <t xml:space="preserve">7000.42</t>
+          <t xml:space="preserve">4989.16</t>
         </is>
       </c>
     </row>
@@ -3810,22 +3810,22 @@
       </c>
       <c s="9" t="inlineStr" r="D82">
         <is>
-          <t xml:space="preserve">11284.00</t>
+          <t xml:space="preserve">13439.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F82">
         <is>
-          <t xml:space="preserve">7898.10</t>
+          <t xml:space="preserve">10907.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G82">
         <is>
-          <t xml:space="preserve">7391.10</t>
+          <t xml:space="preserve">10901.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H82">
         <is>
-          <t xml:space="preserve">7641.10</t>
+          <t xml:space="preserve">10901.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I82">
@@ -3835,12 +3835,12 @@
       </c>
       <c s="9" t="inlineStr" r="J82">
         <is>
-          <t xml:space="preserve">7641.10</t>
+          <t xml:space="preserve">10901.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K82">
         <is>
-          <t xml:space="preserve">7869.05</t>
+          <t xml:space="preserve">7100.19</t>
         </is>
       </c>
     </row>
@@ -3856,22 +3856,22 @@
       </c>
       <c s="9" t="inlineStr" r="D83">
         <is>
-          <t xml:space="preserve">11769.50</t>
+          <t xml:space="preserve">13193.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F83">
         <is>
-          <t xml:space="preserve">8005.90</t>
+          <t xml:space="preserve">10769.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G83">
         <is>
-          <t xml:space="preserve">7498.90</t>
+          <t xml:space="preserve">10769.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H83">
         <is>
-          <t xml:space="preserve">7748.90</t>
+          <t xml:space="preserve">10769.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I83">
@@ -3881,12 +3881,12 @@
       </c>
       <c s="9" t="inlineStr" r="J83">
         <is>
-          <t xml:space="preserve">7748.90</t>
+          <t xml:space="preserve">10769.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K83">
         <is>
-          <t xml:space="preserve">7901.41</t>
+          <t xml:space="preserve">6000.14</t>
         </is>
       </c>
     </row>
@@ -3900,22 +3900,22 @@
       </c>
       <c s="9" t="inlineStr" r="D84">
         <is>
-          <t xml:space="preserve">11310.50</t>
+          <t xml:space="preserve">13177.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F84">
         <is>
-          <t xml:space="preserve">8180.90</t>
+          <t xml:space="preserve">10717.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G84">
         <is>
-          <t xml:space="preserve">7673.90</t>
+          <t xml:space="preserve">10717.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H84">
         <is>
-          <t xml:space="preserve">7863.90</t>
+          <t xml:space="preserve">10717.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I84">
@@ -3925,12 +3925,12 @@
       </c>
       <c s="9" t="inlineStr" r="J84">
         <is>
-          <t xml:space="preserve">7863.90</t>
+          <t xml:space="preserve">10717.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K84">
         <is>
-          <t xml:space="preserve">7000.01</t>
+          <t xml:space="preserve">6000.34</t>
         </is>
       </c>
     </row>
@@ -3944,22 +3944,22 @@
       </c>
       <c s="9" t="inlineStr" r="D85">
         <is>
-          <t xml:space="preserve">10857.00</t>
+          <t xml:space="preserve">13512.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F85">
         <is>
-          <t xml:space="preserve">8389.40</t>
+          <t xml:space="preserve">10737.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G85">
         <is>
-          <t xml:space="preserve">7664.32</t>
+          <t xml:space="preserve">10652.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H85">
         <is>
-          <t xml:space="preserve">7841.80</t>
+          <t xml:space="preserve">10652.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I85">
@@ -3969,12 +3969,12 @@
       </c>
       <c s="9" t="inlineStr" r="J85">
         <is>
-          <t xml:space="preserve">7841.80</t>
+          <t xml:space="preserve">10652.00</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K85">
         <is>
-          <t xml:space="preserve">6469.12</t>
+          <t xml:space="preserve">5902.17</t>
         </is>
       </c>
     </row>
@@ -3988,22 +3988,22 @@
       </c>
       <c s="9" t="inlineStr" r="D86">
         <is>
-          <t xml:space="preserve">10307.60</t>
+          <t xml:space="preserve">13429.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F86">
         <is>
-          <t xml:space="preserve">8605.90</t>
+          <t xml:space="preserve">10668.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G86">
         <is>
-          <t xml:space="preserve">7401.67</t>
+          <t xml:space="preserve">10583.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H86">
         <is>
-          <t xml:space="preserve">7649.70</t>
+          <t xml:space="preserve">10583.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I86">
@@ -4013,12 +4013,12 @@
       </c>
       <c s="9" t="inlineStr" r="J86">
         <is>
-          <t xml:space="preserve">7649.70</t>
+          <t xml:space="preserve">10583.40</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K86">
         <is>
-          <t xml:space="preserve">5469.02</t>
+          <t xml:space="preserve">5812.20</t>
         </is>
       </c>
     </row>
@@ -4034,22 +4034,22 @@
       </c>
       <c s="9" t="inlineStr" r="D87">
         <is>
-          <t xml:space="preserve">9501.10</t>
+          <t xml:space="preserve">12847.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F87">
         <is>
-          <t xml:space="preserve">8075.30</t>
+          <t xml:space="preserve">10850.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G87">
         <is>
-          <t xml:space="preserve">7189.60</t>
+          <t xml:space="preserve">10600.37</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H87">
         <is>
-          <t xml:space="preserve">7435.20</t>
+          <t xml:space="preserve">10590.79</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I87">
@@ -4059,12 +4059,12 @@
       </c>
       <c s="9" t="inlineStr" r="J87">
         <is>
-          <t xml:space="preserve">7435.20</t>
+          <t xml:space="preserve">10590.79</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K87">
         <is>
-          <t xml:space="preserve">5063.41</t>
+          <t xml:space="preserve">5229.40</t>
         </is>
       </c>
     </row>
@@ -4078,22 +4078,22 @@
       </c>
       <c s="9" t="inlineStr" r="D88">
         <is>
-          <t xml:space="preserve">9229.50</t>
+          <t xml:space="preserve">12543.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F88">
         <is>
-          <t xml:space="preserve">7798.50</t>
+          <t xml:space="preserve">10993.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G88">
         <is>
-          <t xml:space="preserve">6913.50</t>
+          <t xml:space="preserve">10462.29</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H88">
         <is>
-          <t xml:space="preserve">7163.50</t>
+          <t xml:space="preserve">10452.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I88">
@@ -4103,12 +4103,12 @@
       </c>
       <c s="9" t="inlineStr" r="J88">
         <is>
-          <t xml:space="preserve">7163.50</t>
+          <t xml:space="preserve">10452.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K88">
         <is>
-          <t xml:space="preserve">4800.26</t>
+          <t xml:space="preserve">4999.23</t>
         </is>
       </c>
     </row>
@@ -4122,22 +4122,22 @@
       </c>
       <c s="9" t="inlineStr" r="D89">
         <is>
-          <t xml:space="preserve">9174.40</t>
+          <t xml:space="preserve">12322.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F89">
         <is>
-          <t xml:space="preserve">7725.50</t>
+          <t xml:space="preserve">11200.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G89">
         <is>
-          <t xml:space="preserve">6618.50</t>
+          <t xml:space="preserve">10439.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H89">
         <is>
-          <t xml:space="preserve">6868.50</t>
+          <t xml:space="preserve">10429.92</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I89">
@@ -4147,12 +4147,12 @@
       </c>
       <c s="9" t="inlineStr" r="J89">
         <is>
-          <t xml:space="preserve">6868.50</t>
+          <t xml:space="preserve">10429.92</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K89">
         <is>
-          <t xml:space="preserve">4500.85</t>
+          <t xml:space="preserve">4729.20</t>
         </is>
       </c>
     </row>
@@ -4166,22 +4166,22 @@
       </c>
       <c s="9" t="inlineStr" r="D90">
         <is>
-          <t xml:space="preserve">9156.30</t>
+          <t xml:space="preserve">11918.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F90">
         <is>
-          <t xml:space="preserve">7803.70</t>
+          <t xml:space="preserve">11206.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G90">
         <is>
-          <t xml:space="preserve">6796.70</t>
+          <t xml:space="preserve">10216.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H90">
         <is>
-          <t xml:space="preserve">7046.70</t>
+          <t xml:space="preserve">10216.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I90">
@@ -4191,12 +4191,12 @@
       </c>
       <c s="9" t="inlineStr" r="J90">
         <is>
-          <t xml:space="preserve">7046.70</t>
+          <t xml:space="preserve">10216.00</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K90">
         <is>
-          <t xml:space="preserve">4500.39</t>
+          <t xml:space="preserve">4500.70</t>
         </is>
       </c>
     </row>
@@ -4212,22 +4212,22 @@
       </c>
       <c s="9" t="inlineStr" r="D91">
         <is>
-          <t xml:space="preserve">8743.80</t>
+          <t xml:space="preserve">11929.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F91">
         <is>
-          <t xml:space="preserve">7364.80</t>
+          <t xml:space="preserve">10827.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G91">
         <is>
-          <t xml:space="preserve">6304.00</t>
+          <t xml:space="preserve">9855.83</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H91">
         <is>
-          <t xml:space="preserve">6439.39</t>
+          <t xml:space="preserve">9846.24</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I91">
@@ -4237,12 +4237,12 @@
       </c>
       <c s="9" t="inlineStr" r="J91">
         <is>
-          <t xml:space="preserve">6439.39</t>
+          <t xml:space="preserve">9846.24</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K91">
         <is>
-          <t xml:space="preserve">4362.26</t>
+          <t xml:space="preserve">4529.07</t>
         </is>
       </c>
     </row>
@@ -4256,22 +4256,22 @@
       </c>
       <c s="9" t="inlineStr" r="D92">
         <is>
-          <t xml:space="preserve">8228.00</t>
+          <t xml:space="preserve">11687.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F92">
         <is>
-          <t xml:space="preserve">7267.40</t>
+          <t xml:space="preserve">10702.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G92">
         <is>
-          <t xml:space="preserve">6141.07</t>
+          <t xml:space="preserve">9716.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H92">
         <is>
-          <t xml:space="preserve">6355.07</t>
+          <t xml:space="preserve">9716.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I92">
@@ -4281,12 +4281,12 @@
       </c>
       <c s="9" t="inlineStr" r="J92">
         <is>
-          <t xml:space="preserve">6355.07</t>
+          <t xml:space="preserve">9716.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K92">
         <is>
-          <t xml:space="preserve">4165.47</t>
+          <t xml:space="preserve">4498.40</t>
         </is>
       </c>
     </row>
@@ -4300,22 +4300,22 @@
       </c>
       <c s="9" t="inlineStr" r="D93">
         <is>
-          <t xml:space="preserve">7962.80</t>
+          <t xml:space="preserve">11079.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F93">
         <is>
-          <t xml:space="preserve">7351.60</t>
+          <t xml:space="preserve">11298.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G93">
         <is>
-          <t xml:space="preserve">6132.50</t>
+          <t xml:space="preserve">9516.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H93">
         <is>
-          <t xml:space="preserve">6284.20</t>
+          <t xml:space="preserve">9516.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I93">
@@ -4325,12 +4325,12 @@
       </c>
       <c s="9" t="inlineStr" r="J93">
         <is>
-          <t xml:space="preserve">6284.20</t>
+          <t xml:space="preserve">9516.00</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K93">
         <is>
-          <t xml:space="preserve">4000.02</t>
+          <t xml:space="preserve">3990.92</t>
         </is>
       </c>
     </row>
@@ -4344,22 +4344,22 @@
       </c>
       <c s="9" t="inlineStr" r="D94">
         <is>
-          <t xml:space="preserve">7993.20</t>
+          <t xml:space="preserve">11061.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F94">
         <is>
-          <t xml:space="preserve">7570.60</t>
+          <t xml:space="preserve">11631.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G94">
         <is>
-          <t xml:space="preserve">6313.80</t>
+          <t xml:space="preserve">9728.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H94">
         <is>
-          <t xml:space="preserve">6435.30</t>
+          <t xml:space="preserve">9718.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I94">
@@ -4369,12 +4369,12 @@
       </c>
       <c s="9" t="inlineStr" r="J94">
         <is>
-          <t xml:space="preserve">6435.30</t>
+          <t xml:space="preserve">9718.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K94">
         <is>
-          <t xml:space="preserve">3822.93</t>
+          <t xml:space="preserve">3659.29</t>
         </is>
       </c>
     </row>
@@ -4390,22 +4390,22 @@
       </c>
       <c s="9" t="inlineStr" r="D95">
         <is>
-          <t xml:space="preserve">7773.30</t>
+          <t xml:space="preserve">10709.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F95">
         <is>
-          <t xml:space="preserve">7760.10</t>
+          <t xml:space="preserve">11101.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G95">
         <is>
-          <t xml:space="preserve">5751.60</t>
+          <t xml:space="preserve">8957.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H95">
         <is>
-          <t xml:space="preserve">5782.90</t>
+          <t xml:space="preserve">8947.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I95">
@@ -4415,12 +4415,12 @@
       </c>
       <c s="9" t="inlineStr" r="J95">
         <is>
-          <t xml:space="preserve">5782.90</t>
+          <t xml:space="preserve">8947.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K95">
         <is>
-          <t xml:space="preserve">3449.55</t>
+          <t xml:space="preserve">3469.72</t>
         </is>
       </c>
     </row>
@@ -4434,22 +4434,22 @@
       </c>
       <c s="9" t="inlineStr" r="D96">
         <is>
-          <t xml:space="preserve">7769.80</t>
+          <t xml:space="preserve">10752.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F96">
         <is>
-          <t xml:space="preserve">7650.10</t>
+          <t xml:space="preserve">10987.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G96">
         <is>
-          <t xml:space="preserve">5637.00</t>
+          <t xml:space="preserve">8928.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H96">
         <is>
-          <t xml:space="preserve">5779.10</t>
+          <t xml:space="preserve">8928.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I96">
@@ -4459,12 +4459,12 @@
       </c>
       <c s="9" t="inlineStr" r="J96">
         <is>
-          <t xml:space="preserve">5779.10</t>
+          <t xml:space="preserve">8928.40</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K96">
         <is>
-          <t xml:space="preserve">3509.42</t>
+          <t xml:space="preserve">3500.51</t>
         </is>
       </c>
     </row>
@@ -4478,22 +4478,22 @@
       </c>
       <c s="9" t="inlineStr" r="D97">
         <is>
-          <t xml:space="preserve">7731.90</t>
+          <t xml:space="preserve">11012.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F97">
         <is>
-          <t xml:space="preserve">7942.30</t>
+          <t xml:space="preserve">10958.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G97">
         <is>
-          <t xml:space="preserve">5716.30</t>
+          <t xml:space="preserve">9136.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H97">
         <is>
-          <t xml:space="preserve">5747.60</t>
+          <t xml:space="preserve">9136.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I97">
@@ -4503,12 +4503,12 @@
       </c>
       <c s="9" t="inlineStr" r="J97">
         <is>
-          <t xml:space="preserve">5747.60</t>
+          <t xml:space="preserve">9136.00</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K97">
         <is>
-          <t xml:space="preserve">3448.51</t>
+          <t xml:space="preserve">3800.74</t>
         </is>
       </c>
     </row>
@@ -4522,22 +4522,22 @@
       </c>
       <c s="9" t="inlineStr" r="D98">
         <is>
-          <t xml:space="preserve">8220.20</t>
+          <t xml:space="preserve">11237.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F98">
         <is>
-          <t xml:space="preserve">8493.20</t>
+          <t xml:space="preserve">11056.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G98">
         <is>
-          <t xml:space="preserve">6202.50</t>
+          <t xml:space="preserve">9252.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H98">
         <is>
-          <t xml:space="preserve">6233.80</t>
+          <t xml:space="preserve">9242.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I98">
@@ -4547,12 +4547,12 @@
       </c>
       <c s="9" t="inlineStr" r="J98">
         <is>
-          <t xml:space="preserve">6233.80</t>
+          <t xml:space="preserve">9242.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K98">
         <is>
-          <t xml:space="preserve">3565.00</t>
+          <t xml:space="preserve">3999.30</t>
         </is>
       </c>
     </row>
@@ -4568,22 +4568,22 @@
       </c>
       <c s="9" t="inlineStr" r="D99">
         <is>
-          <t xml:space="preserve">8220.50</t>
+          <t xml:space="preserve">11047.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F99">
         <is>
-          <t xml:space="preserve">9176.50</t>
+          <t xml:space="preserve">10806.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G99">
         <is>
-          <t xml:space="preserve">6338.80</t>
+          <t xml:space="preserve">8994.22</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H99">
         <is>
-          <t xml:space="preserve">6436.90</t>
+          <t xml:space="preserve">8984.63</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I99">
@@ -4593,12 +4593,12 @@
       </c>
       <c s="9" t="inlineStr" r="J99">
         <is>
-          <t xml:space="preserve">6436.90</t>
+          <t xml:space="preserve">8984.63</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K99">
         <is>
-          <t xml:space="preserve">3509.38</t>
+          <t xml:space="preserve">3664.11</t>
         </is>
       </c>
     </row>
@@ -4612,22 +4612,22 @@
       </c>
       <c s="9" t="inlineStr" r="D100">
         <is>
-          <t xml:space="preserve">8503.00</t>
+          <t xml:space="preserve">10921.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F100">
         <is>
-          <t xml:space="preserve">9830.50</t>
+          <t xml:space="preserve">10906.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G100">
         <is>
-          <t xml:space="preserve">6715.00</t>
+          <t xml:space="preserve">8948.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H100">
         <is>
-          <t xml:space="preserve">6725.30</t>
+          <t xml:space="preserve">8948.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I100">
@@ -4637,12 +4637,12 @@
       </c>
       <c s="9" t="inlineStr" r="J100">
         <is>
-          <t xml:space="preserve">6725.30</t>
+          <t xml:space="preserve">8948.00</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K100">
         <is>
-          <t xml:space="preserve">3442.96</t>
+          <t xml:space="preserve">3500.05</t>
         </is>
       </c>
     </row>
@@ -4656,22 +4656,22 @@
       </c>
       <c s="9" t="inlineStr" r="D101">
         <is>
-          <t xml:space="preserve">8391.30</t>
+          <t xml:space="preserve">11004.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F101">
         <is>
-          <t xml:space="preserve">10343.70</t>
+          <t xml:space="preserve">10874.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G101">
         <is>
-          <t xml:space="preserve">6623.30</t>
+          <t xml:space="preserve">8917.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H101">
         <is>
-          <t xml:space="preserve">6626.50</t>
+          <t xml:space="preserve">8916.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I101">
@@ -4681,12 +4681,12 @@
       </c>
       <c s="9" t="inlineStr" r="J101">
         <is>
-          <t xml:space="preserve">6626.50</t>
+          <t xml:space="preserve">8916.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K101">
         <is>
-          <t xml:space="preserve">3342.54</t>
+          <t xml:space="preserve">3559.10</t>
         </is>
       </c>
     </row>
@@ -4700,22 +4700,22 @@
       </c>
       <c s="9" t="inlineStr" r="D102">
         <is>
-          <t xml:space="preserve">8527.60</t>
+          <t xml:space="preserve">10891.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F102">
         <is>
-          <t xml:space="preserve">10638.10</t>
+          <t xml:space="preserve">10880.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G102">
         <is>
-          <t xml:space="preserve">6753.40</t>
+          <t xml:space="preserve">8922.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H102">
         <is>
-          <t xml:space="preserve">6762.51</t>
+          <t xml:space="preserve">8922.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I102">
@@ -4725,12 +4725,12 @@
       </c>
       <c s="9" t="inlineStr" r="J102">
         <is>
-          <t xml:space="preserve">6762.51</t>
+          <t xml:space="preserve">8922.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K102">
         <is>
-          <t xml:space="preserve">3408.64</t>
+          <t xml:space="preserve">3511.17</t>
         </is>
       </c>
     </row>
@@ -4805,7 +4805,7 @@
     <row r="105" ht="15" customHeight="0">
       <c s="6" t="inlineStr" r="A105">
         <is>
-          <t xml:space="preserve">01-03-2021</t>
+          <t xml:space="preserve">24-03-2021</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="B105">
@@ -4816,22 +4816,22 @@
       <c s="5" t="str" r="C105"/>
       <c s="18" t="inlineStr" r="D105">
         <is>
-          <t xml:space="preserve">233062.60</t>
+          <t xml:space="preserve">294193.75</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="F105">
         <is>
-          <t xml:space="preserve">260662.33</t>
+          <t xml:space="preserve">313216.53</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="G105">
         <is>
-          <t xml:space="preserve">186429.54</t>
+          <t xml:space="preserve">256287.43</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="H105">
         <is>
-          <t xml:space="preserve">185888.56</t>
+          <t xml:space="preserve">251014.49</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="I105">
@@ -4841,7 +4841,7 @@
       </c>
       <c s="18" t="inlineStr" r="J105">
         <is>
-          <t xml:space="preserve">185888.56</t>
+          <t xml:space="preserve">251014.49</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K105">
@@ -4860,22 +4860,22 @@
       <c s="5" t="str" r="C106"/>
       <c s="18" t="inlineStr" r="D106">
         <is>
-          <t xml:space="preserve">13303.90</t>
+          <t xml:space="preserve">15376.50</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="F106">
         <is>
-          <t xml:space="preserve">16023.80</t>
+          <t xml:space="preserve">15913.50</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="G106">
         <is>
-          <t xml:space="preserve">11029.50</t>
+          <t xml:space="preserve">13471.80</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="H106">
         <is>
-          <t xml:space="preserve">11066.78</t>
+          <t xml:space="preserve">13462.20</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="I106">
@@ -4885,12 +4885,12 @@
       </c>
       <c s="18" t="inlineStr" r="J106">
         <is>
-          <t xml:space="preserve">11066.78</t>
+          <t xml:space="preserve">13462.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K106">
         <is>
-          <t xml:space="preserve">7901.41</t>
+          <t xml:space="preserve">7100.19</t>
         </is>
       </c>
     </row>
@@ -4904,22 +4904,22 @@
       <c s="5" t="str" r="C107"/>
       <c s="18" t="inlineStr" r="D107">
         <is>
-          <t xml:space="preserve">7731.90</t>
+          <t xml:space="preserve">10709.10</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="F107">
         <is>
-          <t xml:space="preserve">7267.40</t>
+          <t xml:space="preserve">10588.80</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="G107">
         <is>
-          <t xml:space="preserve">5637.00</t>
+          <t xml:space="preserve">8917.20</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="H107">
         <is>
-          <t xml:space="preserve">5747.60</t>
+          <t xml:space="preserve">8916.20</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="I107">
@@ -4929,12 +4929,12 @@
       </c>
       <c s="18" t="inlineStr" r="J107">
         <is>
-          <t xml:space="preserve">5747.60</t>
+          <t xml:space="preserve">8916.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K107">
         <is>
-          <t xml:space="preserve">2799.71</t>
+          <t xml:space="preserve">2979.75</t>
         </is>
       </c>
     </row>
@@ -4948,22 +4948,22 @@
       <c s="5" t="str" r="C108"/>
       <c s="18" t="inlineStr" r="D108">
         <is>
-          <t xml:space="preserve">9710.94</t>
+          <t xml:space="preserve">12258.07</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="F108">
         <is>
-          <t xml:space="preserve">10860.93</t>
+          <t xml:space="preserve">13050.69</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="G108">
         <is>
-          <t xml:space="preserve">7767.90</t>
+          <t xml:space="preserve">10678.64</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="H108">
         <is>
-          <t xml:space="preserve">7745.36</t>
+          <t xml:space="preserve">10458.94</t>
         </is>
       </c>
       <c s="18" t="inlineStr" r="I108">
@@ -4973,12 +4973,12 @@
       </c>
       <c s="18" t="inlineStr" r="J108">
         <is>
-          <t xml:space="preserve">7745.36</t>
+          <t xml:space="preserve">10458.94</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K108">
         <is>
-          <t xml:space="preserve">4001.35</t>
+          <t xml:space="preserve">3777.89</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
wbes px reports automation done
</commit_message>
<xml_diff>
--- a/Dumps/iexDamFile/MarketMinute.xlsx
+++ b/Dumps/iexDamFile/MarketMinute.xlsx
@@ -377,7 +377,7 @@
     <row r="4" ht="14.4" customHeight="1">
       <c s="2" t="inlineStr" r="A4">
         <is>
-          <t xml:space="preserve">Date: 05-04-2021</t>
+          <t xml:space="preserve">Date: 14-04-2021</t>
         </is>
       </c>
     </row>
@@ -452,7 +452,7 @@
     <row r="7" ht="13.6" customHeight="0">
       <c s="6" t="inlineStr" r="A7">
         <is>
-          <t xml:space="preserve">05-04-2021</t>
+          <t xml:space="preserve">14-04-2021</t>
         </is>
       </c>
       <c s="7" r="B7">
@@ -465,22 +465,22 @@
       </c>
       <c s="9" t="inlineStr" r="D7">
         <is>
-          <t xml:space="preserve">12898.30</t>
+          <t xml:space="preserve">10509.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F7">
         <is>
-          <t xml:space="preserve">10548.40</t>
+          <t xml:space="preserve">6833.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G7">
         <is>
-          <t xml:space="preserve">10199.60</t>
+          <t xml:space="preserve">6709.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H7">
         <is>
-          <t xml:space="preserve">10199.60</t>
+          <t xml:space="preserve">6709.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I7">
@@ -490,12 +490,12 @@
       </c>
       <c s="9" t="inlineStr" r="J7">
         <is>
-          <t xml:space="preserve">10199.60</t>
+          <t xml:space="preserve">6709.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K7">
         <is>
-          <t xml:space="preserve">5650.57</t>
+          <t xml:space="preserve">6500.10</t>
         </is>
       </c>
     </row>
@@ -509,22 +509,22 @@
       </c>
       <c s="9" t="inlineStr" r="D8">
         <is>
-          <t xml:space="preserve">12975.90</t>
+          <t xml:space="preserve">10156.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F8">
         <is>
-          <t xml:space="preserve">10737.10</t>
+          <t xml:space="preserve">6615.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G8">
         <is>
-          <t xml:space="preserve">10382.80</t>
+          <t xml:space="preserve">6441.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H8">
         <is>
-          <t xml:space="preserve">10382.80</t>
+          <t xml:space="preserve">6441.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I8">
@@ -534,12 +534,12 @@
       </c>
       <c s="9" t="inlineStr" r="J8">
         <is>
-          <t xml:space="preserve">10382.80</t>
+          <t xml:space="preserve">6441.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K8">
         <is>
-          <t xml:space="preserve">5580.33</t>
+          <t xml:space="preserve">5900.41</t>
         </is>
       </c>
     </row>
@@ -553,22 +553,22 @@
       </c>
       <c s="9" t="inlineStr" r="D9">
         <is>
-          <t xml:space="preserve">13075.40</t>
+          <t xml:space="preserve">9897.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F9">
         <is>
-          <t xml:space="preserve">10928.80</t>
+          <t xml:space="preserve">6818.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G9">
         <is>
-          <t xml:space="preserve">10566.10</t>
+          <t xml:space="preserve">6554.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H9">
         <is>
-          <t xml:space="preserve">10566.10</t>
+          <t xml:space="preserve">6554.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I9">
@@ -578,12 +578,12 @@
       </c>
       <c s="9" t="inlineStr" r="J9">
         <is>
-          <t xml:space="preserve">10566.10</t>
+          <t xml:space="preserve">6554.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K9">
         <is>
-          <t xml:space="preserve">5580.14</t>
+          <t xml:space="preserve">5000.70</t>
         </is>
       </c>
     </row>
@@ -597,22 +597,22 @@
       </c>
       <c s="9" t="inlineStr" r="D10">
         <is>
-          <t xml:space="preserve">13110.10</t>
+          <t xml:space="preserve">9603.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F10">
         <is>
-          <t xml:space="preserve">10747.50</t>
+          <t xml:space="preserve">7011.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G10">
         <is>
-          <t xml:space="preserve">10373.60</t>
+          <t xml:space="preserve">6708.15</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H10">
         <is>
-          <t xml:space="preserve">10373.60</t>
+          <t xml:space="preserve">6708.15</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I10">
@@ -622,12 +622,12 @@
       </c>
       <c s="9" t="inlineStr" r="J10">
         <is>
-          <t xml:space="preserve">10373.60</t>
+          <t xml:space="preserve">6708.15</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K10">
         <is>
-          <t xml:space="preserve">5580.44</t>
+          <t xml:space="preserve">4999.93</t>
         </is>
       </c>
     </row>
@@ -643,22 +643,22 @@
       </c>
       <c s="9" t="inlineStr" r="D11">
         <is>
-          <t xml:space="preserve">12846.70</t>
+          <t xml:space="preserve">9443.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F11">
         <is>
-          <t xml:space="preserve">10891.50</t>
+          <t xml:space="preserve">7160.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G11">
         <is>
-          <t xml:space="preserve">9976.10</t>
+          <t xml:space="preserve">6319.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H11">
         <is>
-          <t xml:space="preserve">9976.10</t>
+          <t xml:space="preserve">6319.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I11">
@@ -668,12 +668,12 @@
       </c>
       <c s="9" t="inlineStr" r="J11">
         <is>
-          <t xml:space="preserve">9976.10</t>
+          <t xml:space="preserve">6319.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K11">
         <is>
-          <t xml:space="preserve">4611.00</t>
+          <t xml:space="preserve">4500.51</t>
         </is>
       </c>
     </row>
@@ -687,22 +687,22 @@
       </c>
       <c s="9" t="inlineStr" r="D12">
         <is>
-          <t xml:space="preserve">12560.30</t>
+          <t xml:space="preserve">8984.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F12">
         <is>
-          <t xml:space="preserve">11028.00</t>
+          <t xml:space="preserve">6957.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G12">
         <is>
-          <t xml:space="preserve">10098.60</t>
+          <t xml:space="preserve">6088.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H12">
         <is>
-          <t xml:space="preserve">10098.60</t>
+          <t xml:space="preserve">6088.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I12">
@@ -712,12 +712,12 @@
       </c>
       <c s="9" t="inlineStr" r="J12">
         <is>
-          <t xml:space="preserve">10098.60</t>
+          <t xml:space="preserve">6088.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K12">
         <is>
-          <t xml:space="preserve">4610.01</t>
+          <t xml:space="preserve">4500.62</t>
         </is>
       </c>
     </row>
@@ -731,22 +731,22 @@
       </c>
       <c s="9" t="inlineStr" r="D13">
         <is>
-          <t xml:space="preserve">12065.40</t>
+          <t xml:space="preserve">8602.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F13">
         <is>
-          <t xml:space="preserve">11085.10</t>
+          <t xml:space="preserve">7153.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G13">
         <is>
-          <t xml:space="preserve">9750.30</t>
+          <t xml:space="preserve">6217.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H13">
         <is>
-          <t xml:space="preserve">9750.30</t>
+          <t xml:space="preserve">6217.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I13">
@@ -756,12 +756,12 @@
       </c>
       <c s="9" t="inlineStr" r="J13">
         <is>
-          <t xml:space="preserve">9750.30</t>
+          <t xml:space="preserve">6217.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K13">
         <is>
-          <t xml:space="preserve">3999.86</t>
+          <t xml:space="preserve">4475.90</t>
         </is>
       </c>
     </row>
@@ -775,22 +775,22 @@
       </c>
       <c s="9" t="inlineStr" r="D14">
         <is>
-          <t xml:space="preserve">11958.60</t>
+          <t xml:space="preserve">8019.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F14">
         <is>
-          <t xml:space="preserve">11181.10</t>
+          <t xml:space="preserve">7259.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G14">
         <is>
-          <t xml:space="preserve">9733.60</t>
+          <t xml:space="preserve">5860.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H14">
         <is>
-          <t xml:space="preserve">9733.60</t>
+          <t xml:space="preserve">5860.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I14">
@@ -800,12 +800,12 @@
       </c>
       <c s="9" t="inlineStr" r="J14">
         <is>
-          <t xml:space="preserve">9733.60</t>
+          <t xml:space="preserve">5860.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K14">
         <is>
-          <t xml:space="preserve">3600.95</t>
+          <t xml:space="preserve">4165.59</t>
         </is>
       </c>
     </row>
@@ -821,22 +821,22 @@
       </c>
       <c s="9" t="inlineStr" r="D15">
         <is>
-          <t xml:space="preserve">12187.70</t>
+          <t xml:space="preserve">8478.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F15">
         <is>
-          <t xml:space="preserve">11449.40</t>
+          <t xml:space="preserve">8369.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G15">
         <is>
-          <t xml:space="preserve">9937.50</t>
+          <t xml:space="preserve">6453.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H15">
         <is>
-          <t xml:space="preserve">9937.50</t>
+          <t xml:space="preserve">6453.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I15">
@@ -846,12 +846,12 @@
       </c>
       <c s="9" t="inlineStr" r="J15">
         <is>
-          <t xml:space="preserve">9937.50</t>
+          <t xml:space="preserve">6453.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K15">
         <is>
-          <t xml:space="preserve">3526.00</t>
+          <t xml:space="preserve">3718.53</t>
         </is>
       </c>
     </row>
@@ -865,22 +865,22 @@
       </c>
       <c s="9" t="inlineStr" r="D16">
         <is>
-          <t xml:space="preserve">12216.70</t>
+          <t xml:space="preserve">8358.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F16">
         <is>
-          <t xml:space="preserve">11506.40</t>
+          <t xml:space="preserve">8447.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G16">
         <is>
-          <t xml:space="preserve">9808.24</t>
+          <t xml:space="preserve">6294.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H16">
         <is>
-          <t xml:space="preserve">9808.23</t>
+          <t xml:space="preserve">6294.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I16">
@@ -890,12 +890,12 @@
       </c>
       <c s="9" t="inlineStr" r="J16">
         <is>
-          <t xml:space="preserve">9808.23</t>
+          <t xml:space="preserve">6294.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K16">
         <is>
-          <t xml:space="preserve">3600.86</t>
+          <t xml:space="preserve">3718.48</t>
         </is>
       </c>
     </row>
@@ -909,22 +909,22 @@
       </c>
       <c s="9" t="inlineStr" r="D17">
         <is>
-          <t xml:space="preserve">12166.20</t>
+          <t xml:space="preserve">8337.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F17">
         <is>
-          <t xml:space="preserve">11589.40</t>
+          <t xml:space="preserve">8649.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G17">
         <is>
-          <t xml:space="preserve">9801.40</t>
+          <t xml:space="preserve">6312.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H17">
         <is>
-          <t xml:space="preserve">9801.40</t>
+          <t xml:space="preserve">6312.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I17">
@@ -934,12 +934,12 @@
       </c>
       <c s="9" t="inlineStr" r="J17">
         <is>
-          <t xml:space="preserve">9801.40</t>
+          <t xml:space="preserve">6312.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K17">
         <is>
-          <t xml:space="preserve">3876.10</t>
+          <t xml:space="preserve">3718.63</t>
         </is>
       </c>
     </row>
@@ -953,22 +953,22 @@
       </c>
       <c s="9" t="inlineStr" r="D18">
         <is>
-          <t xml:space="preserve">12120.50</t>
+          <t xml:space="preserve">8052.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F18">
         <is>
-          <t xml:space="preserve">11671.40</t>
+          <t xml:space="preserve">8775.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G18">
         <is>
-          <t xml:space="preserve">9863.10</t>
+          <t xml:space="preserve">6039.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H18">
         <is>
-          <t xml:space="preserve">9863.10</t>
+          <t xml:space="preserve">6039.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I18">
@@ -978,12 +978,12 @@
       </c>
       <c s="9" t="inlineStr" r="J18">
         <is>
-          <t xml:space="preserve">9863.10</t>
+          <t xml:space="preserve">6039.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K18">
         <is>
-          <t xml:space="preserve">3559.19</t>
+          <t xml:space="preserve">3648.64</t>
         </is>
       </c>
     </row>
@@ -999,22 +999,22 @@
       </c>
       <c s="9" t="inlineStr" r="D19">
         <is>
-          <t xml:space="preserve">12203.20</t>
+          <t xml:space="preserve">7776.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F19">
         <is>
-          <t xml:space="preserve">12157.40</t>
+          <t xml:space="preserve">8820.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G19">
         <is>
-          <t xml:space="preserve">9990.00</t>
+          <t xml:space="preserve">5746.12</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H19">
         <is>
-          <t xml:space="preserve">9990.00</t>
+          <t xml:space="preserve">5746.12</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I19">
@@ -1024,12 +1024,12 @@
       </c>
       <c s="9" t="inlineStr" r="J19">
         <is>
-          <t xml:space="preserve">9990.00</t>
+          <t xml:space="preserve">5746.12</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K19">
         <is>
-          <t xml:space="preserve">3469.22</t>
+          <t xml:space="preserve">3600.81</t>
         </is>
       </c>
     </row>
@@ -1043,22 +1043,22 @@
       </c>
       <c s="9" t="inlineStr" r="D20">
         <is>
-          <t xml:space="preserve">12321.10</t>
+          <t xml:space="preserve">7756.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F20">
         <is>
-          <t xml:space="preserve">12000.40</t>
+          <t xml:space="preserve">9100.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G20">
         <is>
-          <t xml:space="preserve">10068.13</t>
+          <t xml:space="preserve">5846.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H20">
         <is>
-          <t xml:space="preserve">10068.14</t>
+          <t xml:space="preserve">5846.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I20">
@@ -1068,12 +1068,12 @@
       </c>
       <c s="9" t="inlineStr" r="J20">
         <is>
-          <t xml:space="preserve">10068.14</t>
+          <t xml:space="preserve">5846.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K20">
         <is>
-          <t xml:space="preserve">3500.59</t>
+          <t xml:space="preserve">3379.98</t>
         </is>
       </c>
     </row>
@@ -1087,22 +1087,22 @@
       </c>
       <c s="9" t="inlineStr" r="D21">
         <is>
-          <t xml:space="preserve">12331.30</t>
+          <t xml:space="preserve">7713.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F21">
         <is>
-          <t xml:space="preserve">12134.40</t>
+          <t xml:space="preserve">9329.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G21">
         <is>
-          <t xml:space="preserve">10118.00</t>
+          <t xml:space="preserve">5868.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H21">
         <is>
-          <t xml:space="preserve">10118.00</t>
+          <t xml:space="preserve">5868.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I21">
@@ -1112,12 +1112,12 @@
       </c>
       <c s="9" t="inlineStr" r="J21">
         <is>
-          <t xml:space="preserve">10118.00</t>
+          <t xml:space="preserve">5868.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K21">
         <is>
-          <t xml:space="preserve">3469.72</t>
+          <t xml:space="preserve">3284.99</t>
         </is>
       </c>
     </row>
@@ -1131,22 +1131,22 @@
       </c>
       <c s="9" t="inlineStr" r="D22">
         <is>
-          <t xml:space="preserve">12307.80</t>
+          <t xml:space="preserve">7676.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F22">
         <is>
-          <t xml:space="preserve">12227.40</t>
+          <t xml:space="preserve">9356.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G22">
         <is>
-          <t xml:space="preserve">10094.40</t>
+          <t xml:space="preserve">5832.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H22">
         <is>
-          <t xml:space="preserve">10094.40</t>
+          <t xml:space="preserve">5832.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I22">
@@ -1156,12 +1156,12 @@
       </c>
       <c s="9" t="inlineStr" r="J22">
         <is>
-          <t xml:space="preserve">10094.40</t>
+          <t xml:space="preserve">5832.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K22">
         <is>
-          <t xml:space="preserve">3469.34</t>
+          <t xml:space="preserve">3284.79</t>
         </is>
       </c>
     </row>
@@ -1177,22 +1177,22 @@
       </c>
       <c s="9" t="inlineStr" r="D23">
         <is>
-          <t xml:space="preserve">12708.00</t>
+          <t xml:space="preserve">7887.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F23">
         <is>
-          <t xml:space="preserve">12306.20</t>
+          <t xml:space="preserve">9413.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G23">
         <is>
-          <t xml:space="preserve">10348.10</t>
+          <t xml:space="preserve">6116.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H23">
         <is>
-          <t xml:space="preserve">10348.10</t>
+          <t xml:space="preserve">6116.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I23">
@@ -1202,12 +1202,12 @@
       </c>
       <c s="9" t="inlineStr" r="J23">
         <is>
-          <t xml:space="preserve">10348.10</t>
+          <t xml:space="preserve">6116.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K23">
         <is>
-          <t xml:space="preserve">3469.92</t>
+          <t xml:space="preserve">3445.09</t>
         </is>
       </c>
     </row>
@@ -1221,22 +1221,22 @@
       </c>
       <c s="9" t="inlineStr" r="D24">
         <is>
-          <t xml:space="preserve">13113.40</t>
+          <t xml:space="preserve">8210.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F24">
         <is>
-          <t xml:space="preserve">12129.20</t>
+          <t xml:space="preserve">9262.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G24">
         <is>
-          <t xml:space="preserve">10505.50</t>
+          <t xml:space="preserve">6347.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H24">
         <is>
-          <t xml:space="preserve">10505.50</t>
+          <t xml:space="preserve">6347.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I24">
@@ -1246,12 +1246,12 @@
       </c>
       <c s="9" t="inlineStr" r="J24">
         <is>
-          <t xml:space="preserve">10505.50</t>
+          <t xml:space="preserve">6347.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K24">
         <is>
-          <t xml:space="preserve">3706.21</t>
+          <t xml:space="preserve">3648.26</t>
         </is>
       </c>
     </row>
@@ -1265,22 +1265,22 @@
       </c>
       <c s="9" t="inlineStr" r="D25">
         <is>
-          <t xml:space="preserve">12960.60</t>
+          <t xml:space="preserve">8583.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F25">
         <is>
-          <t xml:space="preserve">12011.10</t>
+          <t xml:space="preserve">9157.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G25">
         <is>
-          <t xml:space="preserve">10487.40</t>
+          <t xml:space="preserve">6719.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H25">
         <is>
-          <t xml:space="preserve">10487.40</t>
+          <t xml:space="preserve">6719.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I25">
@@ -1290,12 +1290,12 @@
       </c>
       <c s="9" t="inlineStr" r="J25">
         <is>
-          <t xml:space="preserve">10487.40</t>
+          <t xml:space="preserve">6719.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K25">
         <is>
-          <t xml:space="preserve">3761.39</t>
+          <t xml:space="preserve">3699.06</t>
         </is>
       </c>
     </row>
@@ -1309,22 +1309,22 @@
       </c>
       <c s="9" t="inlineStr" r="D26">
         <is>
-          <t xml:space="preserve">13024.20</t>
+          <t xml:space="preserve">8739.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F26">
         <is>
-          <t xml:space="preserve">11901.10</t>
+          <t xml:space="preserve">9629.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G26">
         <is>
-          <t xml:space="preserve">10433.90</t>
+          <t xml:space="preserve">6933.56</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H26">
         <is>
-          <t xml:space="preserve">10433.90</t>
+          <t xml:space="preserve">6933.56</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I26">
@@ -1334,12 +1334,12 @@
       </c>
       <c s="9" t="inlineStr" r="J26">
         <is>
-          <t xml:space="preserve">10433.90</t>
+          <t xml:space="preserve">6933.56</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K26">
         <is>
-          <t xml:space="preserve">3876.95</t>
+          <t xml:space="preserve">3500.31</t>
         </is>
       </c>
     </row>
@@ -1355,22 +1355,22 @@
       </c>
       <c s="9" t="inlineStr" r="D27">
         <is>
-          <t xml:space="preserve">13174.70</t>
+          <t xml:space="preserve">9674.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F27">
         <is>
-          <t xml:space="preserve">12274.00</t>
+          <t xml:space="preserve">9738.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G27">
         <is>
-          <t xml:space="preserve">10692.21</t>
+          <t xml:space="preserve">7733.66</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H27">
         <is>
-          <t xml:space="preserve">10692.22</t>
+          <t xml:space="preserve">7733.66</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I27">
@@ -1380,12 +1380,12 @@
       </c>
       <c s="9" t="inlineStr" r="J27">
         <is>
-          <t xml:space="preserve">10692.22</t>
+          <t xml:space="preserve">7733.66</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K27">
         <is>
-          <t xml:space="preserve">3550.28</t>
+          <t xml:space="preserve">3800.84</t>
         </is>
       </c>
     </row>
@@ -1399,22 +1399,22 @@
       </c>
       <c s="9" t="inlineStr" r="D28">
         <is>
-          <t xml:space="preserve">13498.30</t>
+          <t xml:space="preserve">10346.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F28">
         <is>
-          <t xml:space="preserve">12306.90</t>
+          <t xml:space="preserve">9926.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G28">
         <is>
-          <t xml:space="preserve">10772.50</t>
+          <t xml:space="preserve">8084.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H28">
         <is>
-          <t xml:space="preserve">10772.50</t>
+          <t xml:space="preserve">8084.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I28">
@@ -1424,12 +1424,12 @@
       </c>
       <c s="9" t="inlineStr" r="J28">
         <is>
-          <t xml:space="preserve">10772.50</t>
+          <t xml:space="preserve">8084.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K28">
         <is>
-          <t xml:space="preserve">3876.51</t>
+          <t xml:space="preserve">4100.61</t>
         </is>
       </c>
     </row>
@@ -1443,22 +1443,22 @@
       </c>
       <c s="9" t="inlineStr" r="D29">
         <is>
-          <t xml:space="preserve">14035.20</t>
+          <t xml:space="preserve">10675.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F29">
         <is>
-          <t xml:space="preserve">12510.70</t>
+          <t xml:space="preserve">10574.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G29">
         <is>
-          <t xml:space="preserve">11005.40</t>
+          <t xml:space="preserve">8569.86</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H29">
         <is>
-          <t xml:space="preserve">11005.40</t>
+          <t xml:space="preserve">8569.87</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I29">
@@ -1468,12 +1468,12 @@
       </c>
       <c s="9" t="inlineStr" r="J29">
         <is>
-          <t xml:space="preserve">11005.40</t>
+          <t xml:space="preserve">8569.87</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K29">
         <is>
-          <t xml:space="preserve">3900.24</t>
+          <t xml:space="preserve">3800.87</t>
         </is>
       </c>
     </row>
@@ -1487,22 +1487,22 @@
       </c>
       <c s="9" t="inlineStr" r="D30">
         <is>
-          <t xml:space="preserve">14344.10</t>
+          <t xml:space="preserve">10809.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F30">
         <is>
-          <t xml:space="preserve">12509.90</t>
+          <t xml:space="preserve">10871.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G30">
         <is>
-          <t xml:space="preserve">11004.60</t>
+          <t xml:space="preserve">8729.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H30">
         <is>
-          <t xml:space="preserve">11004.60</t>
+          <t xml:space="preserve">8729.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I30">
@@ -1512,12 +1512,12 @@
       </c>
       <c s="9" t="inlineStr" r="J30">
         <is>
-          <t xml:space="preserve">11004.60</t>
+          <t xml:space="preserve">8729.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K30">
         <is>
-          <t xml:space="preserve">3900.72</t>
+          <t xml:space="preserve">3699.75</t>
         </is>
       </c>
     </row>
@@ -1533,22 +1533,22 @@
       </c>
       <c s="9" t="inlineStr" r="D31">
         <is>
-          <t xml:space="preserve">15046.10</t>
+          <t xml:space="preserve">10634.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F31">
         <is>
-          <t xml:space="preserve">12464.10</t>
+          <t xml:space="preserve">10935.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G31">
         <is>
-          <t xml:space="preserve">11470.80</t>
+          <t xml:space="preserve">9145.13</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H31">
         <is>
-          <t xml:space="preserve">11470.80</t>
+          <t xml:space="preserve">9145.13</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I31">
@@ -1558,12 +1558,12 @@
       </c>
       <c s="9" t="inlineStr" r="J31">
         <is>
-          <t xml:space="preserve">11470.80</t>
+          <t xml:space="preserve">9145.13</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K31">
         <is>
-          <t xml:space="preserve">4500.96</t>
+          <t xml:space="preserve">3800.49</t>
         </is>
       </c>
     </row>
@@ -1577,22 +1577,22 @@
       </c>
       <c s="9" t="inlineStr" r="D32">
         <is>
-          <t xml:space="preserve">15371.70</t>
+          <t xml:space="preserve">10884.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F32">
         <is>
-          <t xml:space="preserve">12377.60</t>
+          <t xml:space="preserve">11317.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G32">
         <is>
-          <t xml:space="preserve">11389.30</t>
+          <t xml:space="preserve">9426.44</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H32">
         <is>
-          <t xml:space="preserve">11389.30</t>
+          <t xml:space="preserve">9426.45</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I32">
@@ -1602,12 +1602,12 @@
       </c>
       <c s="9" t="inlineStr" r="J32">
         <is>
-          <t xml:space="preserve">11389.30</t>
+          <t xml:space="preserve">9426.45</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K32">
         <is>
-          <t xml:space="preserve">4550.48</t>
+          <t xml:space="preserve">3800.57</t>
         </is>
       </c>
     </row>
@@ -1621,22 +1621,22 @@
       </c>
       <c s="9" t="inlineStr" r="D33">
         <is>
-          <t xml:space="preserve">15234.10</t>
+          <t xml:space="preserve">11308.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F33">
         <is>
-          <t xml:space="preserve">12395.00</t>
+          <t xml:space="preserve">11622.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G33">
         <is>
-          <t xml:space="preserve">11406.70</t>
+          <t xml:space="preserve">9727.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H33">
         <is>
-          <t xml:space="preserve">11406.70</t>
+          <t xml:space="preserve">9727.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I33">
@@ -1646,12 +1646,12 @@
       </c>
       <c s="9" t="inlineStr" r="J33">
         <is>
-          <t xml:space="preserve">11406.70</t>
+          <t xml:space="preserve">9727.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K33">
         <is>
-          <t xml:space="preserve">4550.74</t>
+          <t xml:space="preserve">3999.37</t>
         </is>
       </c>
     </row>
@@ -1665,22 +1665,22 @@
       </c>
       <c s="9" t="inlineStr" r="D34">
         <is>
-          <t xml:space="preserve">14940.70</t>
+          <t xml:space="preserve">11600.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F34">
         <is>
-          <t xml:space="preserve">12092.40</t>
+          <t xml:space="preserve">11678.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G34">
         <is>
-          <t xml:space="preserve">11104.10</t>
+          <t xml:space="preserve">9850.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H34">
         <is>
-          <t xml:space="preserve">11104.10</t>
+          <t xml:space="preserve">9850.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I34">
@@ -1690,12 +1690,12 @@
       </c>
       <c s="9" t="inlineStr" r="J34">
         <is>
-          <t xml:space="preserve">11104.10</t>
+          <t xml:space="preserve">9850.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K34">
         <is>
-          <t xml:space="preserve">4552.43</t>
+          <t xml:space="preserve">4015.00</t>
         </is>
       </c>
     </row>
@@ -1711,22 +1711,22 @@
       </c>
       <c s="9" t="inlineStr" r="D35">
         <is>
-          <t xml:space="preserve">14537.40</t>
+          <t xml:space="preserve">11530.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F35">
         <is>
-          <t xml:space="preserve">11812.10</t>
+          <t xml:space="preserve">11921.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G35">
         <is>
-          <t xml:space="preserve">10831.60</t>
+          <t xml:space="preserve">9995.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H35">
         <is>
-          <t xml:space="preserve">10831.60</t>
+          <t xml:space="preserve">9995.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I35">
@@ -1736,12 +1736,12 @@
       </c>
       <c s="9" t="inlineStr" r="J35">
         <is>
-          <t xml:space="preserve">10831.60</t>
+          <t xml:space="preserve">9995.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K35">
         <is>
-          <t xml:space="preserve">4589.60</t>
+          <t xml:space="preserve">3899.98</t>
         </is>
       </c>
     </row>
@@ -1755,22 +1755,22 @@
       </c>
       <c s="9" t="inlineStr" r="D36">
         <is>
-          <t xml:space="preserve">13917.40</t>
+          <t xml:space="preserve">11466.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F36">
         <is>
-          <t xml:space="preserve">11808.90</t>
+          <t xml:space="preserve">11993.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G36">
         <is>
-          <t xml:space="preserve">10523.60</t>
+          <t xml:space="preserve">10013.06</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H36">
         <is>
-          <t xml:space="preserve">10523.60</t>
+          <t xml:space="preserve">10013.06</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I36">
@@ -1780,12 +1780,12 @@
       </c>
       <c s="9" t="inlineStr" r="J36">
         <is>
-          <t xml:space="preserve">10523.60</t>
+          <t xml:space="preserve">10013.06</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K36">
         <is>
-          <t xml:space="preserve">4440.77</t>
+          <t xml:space="preserve">3811.34</t>
         </is>
       </c>
     </row>
@@ -1799,22 +1799,22 @@
       </c>
       <c s="9" t="inlineStr" r="D37">
         <is>
-          <t xml:space="preserve">13133.40</t>
+          <t xml:space="preserve">10813.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F37">
         <is>
-          <t xml:space="preserve">11849.40</t>
+          <t xml:space="preserve">12035.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G37">
         <is>
-          <t xml:space="preserve">10427.10</t>
+          <t xml:space="preserve">9785.53</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H37">
         <is>
-          <t xml:space="preserve">10427.10</t>
+          <t xml:space="preserve">9785.53</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I37">
@@ -1824,12 +1824,12 @@
       </c>
       <c s="9" t="inlineStr" r="J37">
         <is>
-          <t xml:space="preserve">10427.10</t>
+          <t xml:space="preserve">9785.53</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K37">
         <is>
-          <t xml:space="preserve">4200.77</t>
+          <t xml:space="preserve">3648.69</t>
         </is>
       </c>
     </row>
@@ -1843,22 +1843,22 @@
       </c>
       <c s="9" t="inlineStr" r="D38">
         <is>
-          <t xml:space="preserve">12644.20</t>
+          <t xml:space="preserve">10370.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F38">
         <is>
-          <t xml:space="preserve">12064.90</t>
+          <t xml:space="preserve">12177.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G38">
         <is>
-          <t xml:space="preserve">10431.60</t>
+          <t xml:space="preserve">9397.94</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H38">
         <is>
-          <t xml:space="preserve">10431.60</t>
+          <t xml:space="preserve">9397.94</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I38">
@@ -1868,12 +1868,12 @@
       </c>
       <c s="9" t="inlineStr" r="J38">
         <is>
-          <t xml:space="preserve">10431.60</t>
+          <t xml:space="preserve">9397.94</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K38">
         <is>
-          <t xml:space="preserve">3518.47</t>
+          <t xml:space="preserve">3569.52</t>
         </is>
       </c>
     </row>
@@ -1889,22 +1889,22 @@
       </c>
       <c s="9" t="inlineStr" r="D39">
         <is>
-          <t xml:space="preserve">11720.70</t>
+          <t xml:space="preserve">9073.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F39">
         <is>
-          <t xml:space="preserve">11861.00</t>
+          <t xml:space="preserve">12190.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G39">
         <is>
-          <t xml:space="preserve">9777.90</t>
+          <t xml:space="preserve">8458.81</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H39">
         <is>
-          <t xml:space="preserve">9777.90</t>
+          <t xml:space="preserve">8458.81</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I39">
@@ -1914,12 +1914,12 @@
       </c>
       <c s="9" t="inlineStr" r="J39">
         <is>
-          <t xml:space="preserve">9777.90</t>
+          <t xml:space="preserve">8458.81</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K39">
         <is>
-          <t xml:space="preserve">3398.19</t>
+          <t xml:space="preserve">2999.38</t>
         </is>
       </c>
     </row>
@@ -1933,22 +1933,22 @@
       </c>
       <c s="9" t="inlineStr" r="D40">
         <is>
-          <t xml:space="preserve">11818.90</t>
+          <t xml:space="preserve">8341.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F40">
         <is>
-          <t xml:space="preserve">11880.40</t>
+          <t xml:space="preserve">12132.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G40">
         <is>
-          <t xml:space="preserve">9976.10</t>
+          <t xml:space="preserve">7924.16</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H40">
         <is>
-          <t xml:space="preserve">9976.10</t>
+          <t xml:space="preserve">7924.17</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I40">
@@ -1958,12 +1958,12 @@
       </c>
       <c s="9" t="inlineStr" r="J40">
         <is>
-          <t xml:space="preserve">9976.10</t>
+          <t xml:space="preserve">7924.17</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K40">
         <is>
-          <t xml:space="preserve">3398.94</t>
+          <t xml:space="preserve">2881.14</t>
         </is>
       </c>
     </row>
@@ -1977,22 +1977,22 @@
       </c>
       <c s="9" t="inlineStr" r="D41">
         <is>
-          <t xml:space="preserve">11866.10</t>
+          <t xml:space="preserve">8235.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F41">
         <is>
-          <t xml:space="preserve">12135.30</t>
+          <t xml:space="preserve">12300.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G41">
         <is>
-          <t xml:space="preserve">10022.80</t>
+          <t xml:space="preserve">7720.71</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H41">
         <is>
-          <t xml:space="preserve">10022.80</t>
+          <t xml:space="preserve">7720.71</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I41">
@@ -2002,12 +2002,12 @@
       </c>
       <c s="9" t="inlineStr" r="J41">
         <is>
-          <t xml:space="preserve">10022.80</t>
+          <t xml:space="preserve">7720.71</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K41">
         <is>
-          <t xml:space="preserve">3398.10</t>
+          <t xml:space="preserve">2969.63</t>
         </is>
       </c>
     </row>
@@ -2021,22 +2021,22 @@
       </c>
       <c s="9" t="inlineStr" r="D42">
         <is>
-          <t xml:space="preserve">11606.90</t>
+          <t xml:space="preserve">7870.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F42">
         <is>
-          <t xml:space="preserve">11963.20</t>
+          <t xml:space="preserve">11230.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G42">
         <is>
-          <t xml:space="preserve">9833.60</t>
+          <t xml:space="preserve">7054.57</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H42">
         <is>
-          <t xml:space="preserve">9833.60</t>
+          <t xml:space="preserve">7054.57</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I42">
@@ -2046,12 +2046,12 @@
       </c>
       <c s="9" t="inlineStr" r="J42">
         <is>
-          <t xml:space="preserve">9833.60</t>
+          <t xml:space="preserve">7054.57</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K42">
         <is>
-          <t xml:space="preserve">3402.40</t>
+          <t xml:space="preserve">3329.17</t>
         </is>
       </c>
     </row>
@@ -2067,22 +2067,22 @@
       </c>
       <c s="9" t="inlineStr" r="D43">
         <is>
-          <t xml:space="preserve">11037.50</t>
+          <t xml:space="preserve">7378.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F43">
         <is>
-          <t xml:space="preserve">11401.10</t>
+          <t xml:space="preserve">10600.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G43">
         <is>
-          <t xml:space="preserve">9372.00</t>
+          <t xml:space="preserve">6416.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H43">
         <is>
-          <t xml:space="preserve">9372.00</t>
+          <t xml:space="preserve">6416.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I43">
@@ -2092,12 +2092,12 @@
       </c>
       <c s="9" t="inlineStr" r="J43">
         <is>
-          <t xml:space="preserve">9372.00</t>
+          <t xml:space="preserve">6416.40</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K43">
         <is>
-          <t xml:space="preserve">3450.43</t>
+          <t xml:space="preserve">3375.55</t>
         </is>
       </c>
     </row>
@@ -2111,22 +2111,22 @@
       </c>
       <c s="9" t="inlineStr" r="D44">
         <is>
-          <t xml:space="preserve">11203.50</t>
+          <t xml:space="preserve">7683.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F44">
         <is>
-          <t xml:space="preserve">10979.40</t>
+          <t xml:space="preserve">10588.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G44">
         <is>
-          <t xml:space="preserve">9374.20</t>
+          <t xml:space="preserve">6584.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H44">
         <is>
-          <t xml:space="preserve">9374.20</t>
+          <t xml:space="preserve">6584.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I44">
@@ -2136,12 +2136,12 @@
       </c>
       <c s="9" t="inlineStr" r="J44">
         <is>
-          <t xml:space="preserve">9374.20</t>
+          <t xml:space="preserve">6584.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K44">
         <is>
-          <t xml:space="preserve">3518.88</t>
+          <t xml:space="preserve">3579.13</t>
         </is>
       </c>
     </row>
@@ -2155,22 +2155,22 @@
       </c>
       <c s="9" t="inlineStr" r="D45">
         <is>
-          <t xml:space="preserve">11246.60</t>
+          <t xml:space="preserve">7591.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F45">
         <is>
-          <t xml:space="preserve">10560.90</t>
+          <t xml:space="preserve">10692.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G45">
         <is>
-          <t xml:space="preserve">9048.40</t>
+          <t xml:space="preserve">6489.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H45">
         <is>
-          <t xml:space="preserve">9048.40</t>
+          <t xml:space="preserve">6489.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I45">
@@ -2180,12 +2180,12 @@
       </c>
       <c s="9" t="inlineStr" r="J45">
         <is>
-          <t xml:space="preserve">9048.40</t>
+          <t xml:space="preserve">6489.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K45">
         <is>
-          <t xml:space="preserve">3920.32</t>
+          <t xml:space="preserve">3579.09</t>
         </is>
       </c>
     </row>
@@ -2199,22 +2199,22 @@
       </c>
       <c s="9" t="inlineStr" r="D46">
         <is>
-          <t xml:space="preserve">11062.40</t>
+          <t xml:space="preserve">7510.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F46">
         <is>
-          <t xml:space="preserve">10925.30</t>
+          <t xml:space="preserve">10911.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G46">
         <is>
-          <t xml:space="preserve">9289.60</t>
+          <t xml:space="preserve">6451.57</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H46">
         <is>
-          <t xml:space="preserve">9289.60</t>
+          <t xml:space="preserve">6451.56</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I46">
@@ -2224,12 +2224,12 @@
       </c>
       <c s="9" t="inlineStr" r="J46">
         <is>
-          <t xml:space="preserve">9289.60</t>
+          <t xml:space="preserve">6451.56</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K46">
         <is>
-          <t xml:space="preserve">3518.66</t>
+          <t xml:space="preserve">3500.41</t>
         </is>
       </c>
     </row>
@@ -2245,22 +2245,22 @@
       </c>
       <c s="9" t="inlineStr" r="D47">
         <is>
-          <t xml:space="preserve">11294.20</t>
+          <t xml:space="preserve">7604.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F47">
         <is>
-          <t xml:space="preserve">11034.80</t>
+          <t xml:space="preserve">11194.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G47">
         <is>
-          <t xml:space="preserve">9362.20</t>
+          <t xml:space="preserve">6345.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H47">
         <is>
-          <t xml:space="preserve">9362.20</t>
+          <t xml:space="preserve">6345.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I47">
@@ -2270,12 +2270,12 @@
       </c>
       <c s="9" t="inlineStr" r="J47">
         <is>
-          <t xml:space="preserve">9362.20</t>
+          <t xml:space="preserve">6345.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K47">
         <is>
-          <t xml:space="preserve">3549.51</t>
+          <t xml:space="preserve">3375.48</t>
         </is>
       </c>
     </row>
@@ -2289,22 +2289,22 @@
       </c>
       <c s="9" t="inlineStr" r="D48">
         <is>
-          <t xml:space="preserve">11603.30</t>
+          <t xml:space="preserve">7761.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F48">
         <is>
-          <t xml:space="preserve">11301.80</t>
+          <t xml:space="preserve">11405.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G48">
         <is>
-          <t xml:space="preserve">9592.75</t>
+          <t xml:space="preserve">6461.76</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H48">
         <is>
-          <t xml:space="preserve">9592.76</t>
+          <t xml:space="preserve">6461.75</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I48">
@@ -2314,12 +2314,12 @@
       </c>
       <c s="9" t="inlineStr" r="J48">
         <is>
-          <t xml:space="preserve">9592.76</t>
+          <t xml:space="preserve">6461.75</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K48">
         <is>
-          <t xml:space="preserve">3600.90</t>
+          <t xml:space="preserve">3500.27</t>
         </is>
       </c>
     </row>
@@ -2333,22 +2333,22 @@
       </c>
       <c s="9" t="inlineStr" r="D49">
         <is>
-          <t xml:space="preserve">11758.40</t>
+          <t xml:space="preserve">7632.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F49">
         <is>
-          <t xml:space="preserve">11519.00</t>
+          <t xml:space="preserve">11855.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G49">
         <is>
-          <t xml:space="preserve">9613.10</t>
+          <t xml:space="preserve">6382.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H49">
         <is>
-          <t xml:space="preserve">9613.10</t>
+          <t xml:space="preserve">6382.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I49">
@@ -2358,12 +2358,12 @@
       </c>
       <c s="9" t="inlineStr" r="J49">
         <is>
-          <t xml:space="preserve">9613.10</t>
+          <t xml:space="preserve">6382.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K49">
         <is>
-          <t xml:space="preserve">3800.44</t>
+          <t xml:space="preserve">3329.11</t>
         </is>
       </c>
     </row>
@@ -2377,22 +2377,22 @@
       </c>
       <c s="9" t="inlineStr" r="D50">
         <is>
-          <t xml:space="preserve">11706.60</t>
+          <t xml:space="preserve">7650.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F50">
         <is>
-          <t xml:space="preserve">12318.30</t>
+          <t xml:space="preserve">11932.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G50">
         <is>
-          <t xml:space="preserve">9881.09</t>
+          <t xml:space="preserve">6425.51</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H50">
         <is>
-          <t xml:space="preserve">9881.09</t>
+          <t xml:space="preserve">6425.51</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I50">
@@ -2402,12 +2402,12 @@
       </c>
       <c s="9" t="inlineStr" r="J50">
         <is>
-          <t xml:space="preserve">9881.09</t>
+          <t xml:space="preserve">6425.51</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K50">
         <is>
-          <t xml:space="preserve">3518.76</t>
+          <t xml:space="preserve">3300.80</t>
         </is>
       </c>
     </row>
@@ -2423,22 +2423,22 @@
       </c>
       <c s="9" t="inlineStr" r="D51">
         <is>
-          <t xml:space="preserve">11942.20</t>
+          <t xml:space="preserve">8144.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F51">
         <is>
-          <t xml:space="preserve">13191.90</t>
+          <t xml:space="preserve">12651.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G51">
         <is>
-          <t xml:space="preserve">10403.95</t>
+          <t xml:space="preserve">7033.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H51">
         <is>
-          <t xml:space="preserve">10403.95</t>
+          <t xml:space="preserve">7033.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I51">
@@ -2448,12 +2448,12 @@
       </c>
       <c s="9" t="inlineStr" r="J51">
         <is>
-          <t xml:space="preserve">10403.95</t>
+          <t xml:space="preserve">7033.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K51">
         <is>
-          <t xml:space="preserve">3450.21</t>
+          <t xml:space="preserve">3151.97</t>
         </is>
       </c>
     </row>
@@ -2467,22 +2467,22 @@
       </c>
       <c s="9" t="inlineStr" r="D52">
         <is>
-          <t xml:space="preserve">11995.00</t>
+          <t xml:space="preserve">8200.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F52">
         <is>
-          <t xml:space="preserve">13796.30</t>
+          <t xml:space="preserve">13554.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G52">
         <is>
-          <t xml:space="preserve">10499.80</t>
+          <t xml:space="preserve">7309.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H52">
         <is>
-          <t xml:space="preserve">10499.80</t>
+          <t xml:space="preserve">7309.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I52">
@@ -2492,12 +2492,12 @@
       </c>
       <c s="9" t="inlineStr" r="J52">
         <is>
-          <t xml:space="preserve">10499.80</t>
+          <t xml:space="preserve">7309.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K52">
         <is>
-          <t xml:space="preserve">3335.77</t>
+          <t xml:space="preserve">3063.58</t>
         </is>
       </c>
     </row>
@@ -2511,22 +2511,22 @@
       </c>
       <c s="9" t="inlineStr" r="D53">
         <is>
-          <t xml:space="preserve">11690.20</t>
+          <t xml:space="preserve">8188.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F53">
         <is>
-          <t xml:space="preserve">14298.30</t>
+          <t xml:space="preserve">14268.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G53">
         <is>
-          <t xml:space="preserve">10211.90</t>
+          <t xml:space="preserve">7390.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H53">
         <is>
-          <t xml:space="preserve">10211.90</t>
+          <t xml:space="preserve">7390.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I53">
@@ -2536,12 +2536,12 @@
       </c>
       <c s="9" t="inlineStr" r="J53">
         <is>
-          <t xml:space="preserve">10211.90</t>
+          <t xml:space="preserve">7390.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K53">
         <is>
-          <t xml:space="preserve">3239.38</t>
+          <t xml:space="preserve">2999.82</t>
         </is>
       </c>
     </row>
@@ -2555,22 +2555,22 @@
       </c>
       <c s="9" t="inlineStr" r="D54">
         <is>
-          <t xml:space="preserve">11609.50</t>
+          <t xml:space="preserve">8014.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F54">
         <is>
-          <t xml:space="preserve">14896.70</t>
+          <t xml:space="preserve">14472.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G54">
         <is>
-          <t xml:space="preserve">10260.00</t>
+          <t xml:space="preserve">7334.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H54">
         <is>
-          <t xml:space="preserve">10260.00</t>
+          <t xml:space="preserve">7334.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I54">
@@ -2580,12 +2580,12 @@
       </c>
       <c s="9" t="inlineStr" r="J54">
         <is>
-          <t xml:space="preserve">10260.00</t>
+          <t xml:space="preserve">7334.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K54">
         <is>
-          <t xml:space="preserve">3199.63</t>
+          <t xml:space="preserve">2866.21</t>
         </is>
       </c>
     </row>
@@ -2601,22 +2601,22 @@
       </c>
       <c s="9" t="inlineStr" r="D55">
         <is>
-          <t xml:space="preserve">11391.70</t>
+          <t xml:space="preserve">7889.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F55">
         <is>
-          <t xml:space="preserve">14862.50</t>
+          <t xml:space="preserve">15469.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G55">
         <is>
-          <t xml:space="preserve">10177.60</t>
+          <t xml:space="preserve">7282.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H55">
         <is>
-          <t xml:space="preserve">10177.60</t>
+          <t xml:space="preserve">7282.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I55">
@@ -2626,12 +2626,12 @@
       </c>
       <c s="9" t="inlineStr" r="J55">
         <is>
-          <t xml:space="preserve">10177.60</t>
+          <t xml:space="preserve">7282.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K55">
         <is>
-          <t xml:space="preserve">3131.72</t>
+          <t xml:space="preserve">2773.18</t>
         </is>
       </c>
     </row>
@@ -2645,22 +2645,22 @@
       </c>
       <c s="9" t="inlineStr" r="D56">
         <is>
-          <t xml:space="preserve">11416.50</t>
+          <t xml:space="preserve">7928.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F56">
         <is>
-          <t xml:space="preserve">15352.00</t>
+          <t xml:space="preserve">15031.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G56">
         <is>
-          <t xml:space="preserve">10202.30</t>
+          <t xml:space="preserve">7321.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H56">
         <is>
-          <t xml:space="preserve">10202.30</t>
+          <t xml:space="preserve">7321.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I56">
@@ -2670,12 +2670,12 @@
       </c>
       <c s="9" t="inlineStr" r="J56">
         <is>
-          <t xml:space="preserve">10202.30</t>
+          <t xml:space="preserve">7321.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K56">
         <is>
-          <t xml:space="preserve">3131.06</t>
+          <t xml:space="preserve">2742.95</t>
         </is>
       </c>
     </row>
@@ -2689,22 +2689,22 @@
       </c>
       <c s="9" t="inlineStr" r="D57">
         <is>
-          <t xml:space="preserve">11351.80</t>
+          <t xml:space="preserve">7503.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F57">
         <is>
-          <t xml:space="preserve">15600.70</t>
+          <t xml:space="preserve">14895.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G57">
         <is>
-          <t xml:space="preserve">10166.90</t>
+          <t xml:space="preserve">6950.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H57">
         <is>
-          <t xml:space="preserve">10166.90</t>
+          <t xml:space="preserve">6950.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I57">
@@ -2714,12 +2714,12 @@
       </c>
       <c s="9" t="inlineStr" r="J57">
         <is>
-          <t xml:space="preserve">10166.90</t>
+          <t xml:space="preserve">6950.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K57">
         <is>
-          <t xml:space="preserve">3065.39</t>
+          <t xml:space="preserve">2668.81</t>
         </is>
       </c>
     </row>
@@ -2733,22 +2733,22 @@
       </c>
       <c s="9" t="inlineStr" r="D58">
         <is>
-          <t xml:space="preserve">11207.20</t>
+          <t xml:space="preserve">7317.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F58">
         <is>
-          <t xml:space="preserve">15758.30</t>
+          <t xml:space="preserve">14993.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G58">
         <is>
-          <t xml:space="preserve">10028.40</t>
+          <t xml:space="preserve">6871.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H58">
         <is>
-          <t xml:space="preserve">10028.40</t>
+          <t xml:space="preserve">6871.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I58">
@@ -2758,12 +2758,12 @@
       </c>
       <c s="9" t="inlineStr" r="J58">
         <is>
-          <t xml:space="preserve">10028.40</t>
+          <t xml:space="preserve">6871.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K58">
         <is>
-          <t xml:space="preserve">3059.67</t>
+          <t xml:space="preserve">2559.96</t>
         </is>
       </c>
     </row>
@@ -2779,22 +2779,22 @@
       </c>
       <c s="9" t="inlineStr" r="D59">
         <is>
-          <t xml:space="preserve">11150.40</t>
+          <t xml:space="preserve">7009.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F59">
         <is>
-          <t xml:space="preserve">16419.70</t>
+          <t xml:space="preserve">15553.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G59">
         <is>
-          <t xml:space="preserve">10004.80</t>
+          <t xml:space="preserve">6563.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H59">
         <is>
-          <t xml:space="preserve">10004.80</t>
+          <t xml:space="preserve">6563.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I59">
@@ -2804,12 +2804,12 @@
       </c>
       <c s="9" t="inlineStr" r="J59">
         <is>
-          <t xml:space="preserve">10004.80</t>
+          <t xml:space="preserve">6563.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K59">
         <is>
-          <t xml:space="preserve">3043.75</t>
+          <t xml:space="preserve">2546.60</t>
         </is>
       </c>
     </row>
@@ -2823,22 +2823,22 @@
       </c>
       <c s="9" t="inlineStr" r="D60">
         <is>
-          <t xml:space="preserve">11051.00</t>
+          <t xml:space="preserve">7197.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F60">
         <is>
-          <t xml:space="preserve">16460.40</t>
+          <t xml:space="preserve">15444.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G60">
         <is>
-          <t xml:space="preserve">9971.20</t>
+          <t xml:space="preserve">6751.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H60">
         <is>
-          <t xml:space="preserve">9971.20</t>
+          <t xml:space="preserve">6751.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I60">
@@ -2848,12 +2848,12 @@
       </c>
       <c s="9" t="inlineStr" r="J60">
         <is>
-          <t xml:space="preserve">9971.20</t>
+          <t xml:space="preserve">6751.90</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K60">
         <is>
-          <t xml:space="preserve">2979.49</t>
+          <t xml:space="preserve">2546.88</t>
         </is>
       </c>
     </row>
@@ -2867,22 +2867,22 @@
       </c>
       <c s="9" t="inlineStr" r="D61">
         <is>
-          <t xml:space="preserve">10955.60</t>
+          <t xml:space="preserve">7357.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F61">
         <is>
-          <t xml:space="preserve">16344.50</t>
+          <t xml:space="preserve">15321.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G61">
         <is>
-          <t xml:space="preserve">10084.40</t>
+          <t xml:space="preserve">6911.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H61">
         <is>
-          <t xml:space="preserve">10084.40</t>
+          <t xml:space="preserve">6911.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I61">
@@ -2892,12 +2892,12 @@
       </c>
       <c s="9" t="inlineStr" r="J61">
         <is>
-          <t xml:space="preserve">10084.40</t>
+          <t xml:space="preserve">6911.40</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K61">
         <is>
-          <t xml:space="preserve">2979.47</t>
+          <t xml:space="preserve">2546.81</t>
         </is>
       </c>
     </row>
@@ -2911,22 +2911,22 @@
       </c>
       <c s="9" t="inlineStr" r="D62">
         <is>
-          <t xml:space="preserve">11059.20</t>
+          <t xml:space="preserve">7223.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F62">
         <is>
-          <t xml:space="preserve">16182.40</t>
+          <t xml:space="preserve">15254.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G62">
         <is>
-          <t xml:space="preserve">10188.00</t>
+          <t xml:space="preserve">6777.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H62">
         <is>
-          <t xml:space="preserve">10188.00</t>
+          <t xml:space="preserve">6777.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I62">
@@ -2936,12 +2936,12 @@
       </c>
       <c s="9" t="inlineStr" r="J62">
         <is>
-          <t xml:space="preserve">10188.00</t>
+          <t xml:space="preserve">6777.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K62">
         <is>
-          <t xml:space="preserve">2979.75</t>
+          <t xml:space="preserve">2546.50</t>
         </is>
       </c>
     </row>
@@ -2957,22 +2957,22 @@
       </c>
       <c s="9" t="inlineStr" r="D63">
         <is>
-          <t xml:space="preserve">11450.70</t>
+          <t xml:space="preserve">7578.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F63">
         <is>
-          <t xml:space="preserve">15718.60</t>
+          <t xml:space="preserve">15015.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G63">
         <is>
-          <t xml:space="preserve">10373.40</t>
+          <t xml:space="preserve">7123.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H63">
         <is>
-          <t xml:space="preserve">10373.40</t>
+          <t xml:space="preserve">7123.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I63">
@@ -2982,12 +2982,12 @@
       </c>
       <c s="9" t="inlineStr" r="J63">
         <is>
-          <t xml:space="preserve">10373.40</t>
+          <t xml:space="preserve">7123.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K63">
         <is>
-          <t xml:space="preserve">3043.88</t>
+          <t xml:space="preserve">2546.67</t>
         </is>
       </c>
     </row>
@@ -3001,22 +3001,22 @@
       </c>
       <c s="9" t="inlineStr" r="D64">
         <is>
-          <t xml:space="preserve">11938.60</t>
+          <t xml:space="preserve">8346.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F64">
         <is>
-          <t xml:space="preserve">15385.40</t>
+          <t xml:space="preserve">14519.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G64">
         <is>
-          <t xml:space="preserve">10849.20</t>
+          <t xml:space="preserve">7828.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H64">
         <is>
-          <t xml:space="preserve">10849.20</t>
+          <t xml:space="preserve">7828.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I64">
@@ -3026,12 +3026,12 @@
       </c>
       <c s="9" t="inlineStr" r="J64">
         <is>
-          <t xml:space="preserve">10849.20</t>
+          <t xml:space="preserve">7828.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K64">
         <is>
-          <t xml:space="preserve">3059.92</t>
+          <t xml:space="preserve">2742.63</t>
         </is>
       </c>
     </row>
@@ -3045,22 +3045,22 @@
       </c>
       <c s="9" t="inlineStr" r="D65">
         <is>
-          <t xml:space="preserve">12512.20</t>
+          <t xml:space="preserve">8439.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F65">
         <is>
-          <t xml:space="preserve">15091.30</t>
+          <t xml:space="preserve">14371.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G65">
         <is>
-          <t xml:space="preserve">11270.80</t>
+          <t xml:space="preserve">7921.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H65">
         <is>
-          <t xml:space="preserve">11270.80</t>
+          <t xml:space="preserve">7921.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I65">
@@ -3070,12 +3070,12 @@
       </c>
       <c s="9" t="inlineStr" r="J65">
         <is>
-          <t xml:space="preserve">11270.80</t>
+          <t xml:space="preserve">7921.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K65">
         <is>
-          <t xml:space="preserve">3150.84</t>
+          <t xml:space="preserve">2742.71</t>
         </is>
       </c>
     </row>
@@ -3089,22 +3089,22 @@
       </c>
       <c s="9" t="inlineStr" r="D66">
         <is>
-          <t xml:space="preserve">12940.00</t>
+          <t xml:space="preserve">9099.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F66">
         <is>
-          <t xml:space="preserve">14778.00</t>
+          <t xml:space="preserve">13967.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G66">
         <is>
-          <t xml:space="preserve">11589.70</t>
+          <t xml:space="preserve">8460.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H66">
         <is>
-          <t xml:space="preserve">11589.70</t>
+          <t xml:space="preserve">8460.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I66">
@@ -3114,12 +3114,12 @@
       </c>
       <c s="9" t="inlineStr" r="J66">
         <is>
-          <t xml:space="preserve">11589.70</t>
+          <t xml:space="preserve">8460.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K66">
         <is>
-          <t xml:space="preserve">3294.05</t>
+          <t xml:space="preserve">2900.90</t>
         </is>
       </c>
     </row>
@@ -3135,22 +3135,22 @@
       </c>
       <c s="9" t="inlineStr" r="D67">
         <is>
-          <t xml:space="preserve">13396.40</t>
+          <t xml:space="preserve">9520.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F67">
         <is>
-          <t xml:space="preserve">14714.30</t>
+          <t xml:space="preserve">13696.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G67">
         <is>
-          <t xml:space="preserve">12027.90</t>
+          <t xml:space="preserve">8723.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H67">
         <is>
-          <t xml:space="preserve">12027.90</t>
+          <t xml:space="preserve">8723.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I67">
@@ -3160,12 +3160,12 @@
       </c>
       <c s="9" t="inlineStr" r="J67">
         <is>
-          <t xml:space="preserve">12027.90</t>
+          <t xml:space="preserve">8723.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K67">
         <is>
-          <t xml:space="preserve">3398.54</t>
+          <t xml:space="preserve">3043.17</t>
         </is>
       </c>
     </row>
@@ -3179,22 +3179,22 @@
       </c>
       <c s="9" t="inlineStr" r="D68">
         <is>
-          <t xml:space="preserve">13002.70</t>
+          <t xml:space="preserve">9748.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F68">
         <is>
-          <t xml:space="preserve">14594.30</t>
+          <t xml:space="preserve">13383.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G68">
         <is>
-          <t xml:space="preserve">11634.90</t>
+          <t xml:space="preserve">8951.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H68">
         <is>
-          <t xml:space="preserve">11634.90</t>
+          <t xml:space="preserve">8951.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I68">
@@ -3204,12 +3204,12 @@
       </c>
       <c s="9" t="inlineStr" r="J68">
         <is>
-          <t xml:space="preserve">11634.90</t>
+          <t xml:space="preserve">8951.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K68">
         <is>
-          <t xml:space="preserve">3363.00</t>
+          <t xml:space="preserve">3043.79</t>
         </is>
       </c>
     </row>
@@ -3223,22 +3223,22 @@
       </c>
       <c s="9" t="inlineStr" r="D69">
         <is>
-          <t xml:space="preserve">12630.50</t>
+          <t xml:space="preserve">10425.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F69">
         <is>
-          <t xml:space="preserve">14367.60</t>
+          <t xml:space="preserve">13006.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G69">
         <is>
-          <t xml:space="preserve">11171.00</t>
+          <t xml:space="preserve">9414.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H69">
         <is>
-          <t xml:space="preserve">11171.00</t>
+          <t xml:space="preserve">9414.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I69">
@@ -3248,12 +3248,12 @@
       </c>
       <c s="9" t="inlineStr" r="J69">
         <is>
-          <t xml:space="preserve">11171.00</t>
+          <t xml:space="preserve">9414.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K69">
         <is>
-          <t xml:space="preserve">3279.46</t>
+          <t xml:space="preserve">3329.74</t>
         </is>
       </c>
     </row>
@@ -3267,22 +3267,22 @@
       </c>
       <c s="9" t="inlineStr" r="D70">
         <is>
-          <t xml:space="preserve">13143.10</t>
+          <t xml:space="preserve">10348.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F70">
         <is>
-          <t xml:space="preserve">14154.70</t>
+          <t xml:space="preserve">12718.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G70">
         <is>
-          <t xml:space="preserve">11581.95</t>
+          <t xml:space="preserve">9337.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H70">
         <is>
-          <t xml:space="preserve">11581.96</t>
+          <t xml:space="preserve">9337.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I70">
@@ -3292,12 +3292,12 @@
       </c>
       <c s="9" t="inlineStr" r="J70">
         <is>
-          <t xml:space="preserve">11581.96</t>
+          <t xml:space="preserve">9337.80</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K70">
         <is>
-          <t xml:space="preserve">3400.85</t>
+          <t xml:space="preserve">3329.49</t>
         </is>
       </c>
     </row>
@@ -3313,22 +3313,22 @@
       </c>
       <c s="9" t="inlineStr" r="D71">
         <is>
-          <t xml:space="preserve">13134.70</t>
+          <t xml:space="preserve">10854.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F71">
         <is>
-          <t xml:space="preserve">13711.90</t>
+          <t xml:space="preserve">12640.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G71">
         <is>
-          <t xml:space="preserve">11508.47</t>
+          <t xml:space="preserve">9818.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H71">
         <is>
-          <t xml:space="preserve">11508.47</t>
+          <t xml:space="preserve">9818.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I71">
@@ -3338,12 +3338,12 @@
       </c>
       <c s="9" t="inlineStr" r="J71">
         <is>
-          <t xml:space="preserve">11508.47</t>
+          <t xml:space="preserve">9818.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K71">
         <is>
-          <t xml:space="preserve">3500.44</t>
+          <t xml:space="preserve">3400.35</t>
         </is>
       </c>
     </row>
@@ -3357,22 +3357,22 @@
       </c>
       <c s="9" t="inlineStr" r="D72">
         <is>
-          <t xml:space="preserve">13637.30</t>
+          <t xml:space="preserve">10900.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F72">
         <is>
-          <t xml:space="preserve">13328.80</t>
+          <t xml:space="preserve">12665.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G72">
         <is>
-          <t xml:space="preserve">11713.50</t>
+          <t xml:space="preserve">9843.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H72">
         <is>
-          <t xml:space="preserve">11713.50</t>
+          <t xml:space="preserve">9843.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I72">
@@ -3382,12 +3382,12 @@
       </c>
       <c s="9" t="inlineStr" r="J72">
         <is>
-          <t xml:space="preserve">11713.50</t>
+          <t xml:space="preserve">9843.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K72">
         <is>
-          <t xml:space="preserve">3700.48</t>
+          <t xml:space="preserve">3500.01</t>
         </is>
       </c>
     </row>
@@ -3401,22 +3401,22 @@
       </c>
       <c s="9" t="inlineStr" r="D73">
         <is>
-          <t xml:space="preserve">13498.30</t>
+          <t xml:space="preserve">10491.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F73">
         <is>
-          <t xml:space="preserve">13040.80</t>
+          <t xml:space="preserve">12768.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G73">
         <is>
-          <t xml:space="preserve">11591.63</t>
+          <t xml:space="preserve">9485.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H73">
         <is>
-          <t xml:space="preserve">11591.64</t>
+          <t xml:space="preserve">9485.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I73">
@@ -3426,12 +3426,12 @@
       </c>
       <c s="9" t="inlineStr" r="J73">
         <is>
-          <t xml:space="preserve">11591.64</t>
+          <t xml:space="preserve">9485.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K73">
         <is>
-          <t xml:space="preserve">3570.46</t>
+          <t xml:space="preserve">3269.31</t>
         </is>
       </c>
     </row>
@@ -3445,22 +3445,22 @@
       </c>
       <c s="9" t="inlineStr" r="D74">
         <is>
-          <t xml:space="preserve">13427.80</t>
+          <t xml:space="preserve">10435.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F74">
         <is>
-          <t xml:space="preserve">12613.80</t>
+          <t xml:space="preserve">12691.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G74">
         <is>
-          <t xml:space="preserve">11328.00</t>
+          <t xml:space="preserve">9430.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H74">
         <is>
-          <t xml:space="preserve">11328.00</t>
+          <t xml:space="preserve">9430.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I74">
@@ -3470,12 +3470,12 @@
       </c>
       <c s="9" t="inlineStr" r="J74">
         <is>
-          <t xml:space="preserve">11328.00</t>
+          <t xml:space="preserve">9430.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K74">
         <is>
-          <t xml:space="preserve">4001.00</t>
+          <t xml:space="preserve">3269.75</t>
         </is>
       </c>
     </row>
@@ -3491,22 +3491,22 @@
       </c>
       <c s="9" t="inlineStr" r="D75">
         <is>
-          <t xml:space="preserve">12356.50</t>
+          <t xml:space="preserve">9183.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F75">
         <is>
-          <t xml:space="preserve">12091.20</t>
+          <t xml:space="preserve">13387.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G75">
         <is>
-          <t xml:space="preserve">10603.80</t>
+          <t xml:space="preserve">8647.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H75">
         <is>
-          <t xml:space="preserve">10603.80</t>
+          <t xml:space="preserve">8647.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I75">
@@ -3516,12 +3516,12 @@
       </c>
       <c s="9" t="inlineStr" r="J75">
         <is>
-          <t xml:space="preserve">10603.80</t>
+          <t xml:space="preserve">8647.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K75">
         <is>
-          <t xml:space="preserve">3469.65</t>
+          <t xml:space="preserve">2742.69</t>
         </is>
       </c>
     </row>
@@ -3535,22 +3535,22 @@
       </c>
       <c s="9" t="inlineStr" r="D76">
         <is>
-          <t xml:space="preserve">12718.10</t>
+          <t xml:space="preserve">9056.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F76">
         <is>
-          <t xml:space="preserve">11003.50</t>
+          <t xml:space="preserve">12384.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G76">
         <is>
-          <t xml:space="preserve">10254.30</t>
+          <t xml:space="preserve">8355.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H76">
         <is>
-          <t xml:space="preserve">10254.30</t>
+          <t xml:space="preserve">8355.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I76">
@@ -3560,12 +3560,12 @@
       </c>
       <c s="9" t="inlineStr" r="J76">
         <is>
-          <t xml:space="preserve">10254.30</t>
+          <t xml:space="preserve">8355.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K76">
         <is>
-          <t xml:space="preserve">4930.01</t>
+          <t xml:space="preserve">2999.53</t>
         </is>
       </c>
     </row>
@@ -3579,22 +3579,22 @@
       </c>
       <c s="9" t="inlineStr" r="D77">
         <is>
-          <t xml:space="preserve">12171.90</t>
+          <t xml:space="preserve">9160.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F77">
         <is>
-          <t xml:space="preserve">10457.00</t>
+          <t xml:space="preserve">11685.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G77">
         <is>
-          <t xml:space="preserve">9722.60</t>
+          <t xml:space="preserve">8199.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H77">
         <is>
-          <t xml:space="preserve">9722.60</t>
+          <t xml:space="preserve">8199.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I77">
@@ -3604,12 +3604,12 @@
       </c>
       <c s="9" t="inlineStr" r="J77">
         <is>
-          <t xml:space="preserve">9722.60</t>
+          <t xml:space="preserve">8199.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K77">
         <is>
-          <t xml:space="preserve">4930.80</t>
+          <t xml:space="preserve">3250.30</t>
         </is>
       </c>
     </row>
@@ -3623,22 +3623,22 @@
       </c>
       <c s="9" t="inlineStr" r="D78">
         <is>
-          <t xml:space="preserve">11965.30</t>
+          <t xml:space="preserve">9302.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F78">
         <is>
-          <t xml:space="preserve">9977.50</t>
+          <t xml:space="preserve">11711.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G78">
         <is>
-          <t xml:space="preserve">9566.10</t>
+          <t xml:space="preserve">8322.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H78">
         <is>
-          <t xml:space="preserve">9566.10</t>
+          <t xml:space="preserve">8322.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I78">
@@ -3648,12 +3648,12 @@
       </c>
       <c s="9" t="inlineStr" r="J78">
         <is>
-          <t xml:space="preserve">9566.10</t>
+          <t xml:space="preserve">8322.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K78">
         <is>
-          <t xml:space="preserve">5000.20</t>
+          <t xml:space="preserve">3349.79</t>
         </is>
       </c>
     </row>
@@ -3669,22 +3669,22 @@
       </c>
       <c s="9" t="inlineStr" r="D79">
         <is>
-          <t xml:space="preserve">10704.30</t>
+          <t xml:space="preserve">8093.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F79">
         <is>
-          <t xml:space="preserve">9821.20</t>
+          <t xml:space="preserve">10838.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G79">
         <is>
-          <t xml:space="preserve">9012.00</t>
+          <t xml:space="preserve">7308.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H79">
         <is>
-          <t xml:space="preserve">9012.00</t>
+          <t xml:space="preserve">7308.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I79">
@@ -3694,12 +3694,12 @@
       </c>
       <c s="9" t="inlineStr" r="J79">
         <is>
-          <t xml:space="preserve">9012.00</t>
+          <t xml:space="preserve">7308.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K79">
         <is>
-          <t xml:space="preserve">4524.00</t>
+          <t xml:space="preserve">3108.78</t>
         </is>
       </c>
     </row>
@@ -3713,22 +3713,22 @@
       </c>
       <c s="9" t="inlineStr" r="D80">
         <is>
-          <t xml:space="preserve">10635.90</t>
+          <t xml:space="preserve">8722.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F80">
         <is>
-          <t xml:space="preserve">9422.60</t>
+          <t xml:space="preserve">10819.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G80">
         <is>
-          <t xml:space="preserve">8598.40</t>
+          <t xml:space="preserve">7758.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H80">
         <is>
-          <t xml:space="preserve">8598.40</t>
+          <t xml:space="preserve">7758.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I80">
@@ -3738,12 +3738,12 @@
       </c>
       <c s="9" t="inlineStr" r="J80">
         <is>
-          <t xml:space="preserve">8598.40</t>
+          <t xml:space="preserve">7758.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K80">
         <is>
-          <t xml:space="preserve">4845.85</t>
+          <t xml:space="preserve">3629.63</t>
         </is>
       </c>
     </row>
@@ -3757,22 +3757,22 @@
       </c>
       <c s="9" t="inlineStr" r="D81">
         <is>
-          <t xml:space="preserve">11563.20</t>
+          <t xml:space="preserve">9670.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F81">
         <is>
-          <t xml:space="preserve">8871.50</t>
+          <t xml:space="preserve">10642.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G81">
         <is>
-          <t xml:space="preserve">8584.50</t>
+          <t xml:space="preserve">8388.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H81">
         <is>
-          <t xml:space="preserve">8584.50</t>
+          <t xml:space="preserve">8388.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I81">
@@ -3782,12 +3782,12 @@
       </c>
       <c s="9" t="inlineStr" r="J81">
         <is>
-          <t xml:space="preserve">8584.50</t>
+          <t xml:space="preserve">8388.00</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K81">
         <is>
-          <t xml:space="preserve">5900.48</t>
+          <t xml:space="preserve">4094.62</t>
         </is>
       </c>
     </row>
@@ -3801,22 +3801,22 @@
       </c>
       <c s="9" t="inlineStr" r="D82">
         <is>
-          <t xml:space="preserve">11491.30</t>
+          <t xml:space="preserve">9766.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F82">
         <is>
-          <t xml:space="preserve">9061.10</t>
+          <t xml:space="preserve">10173.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G82">
         <is>
-          <t xml:space="preserve">8784.10</t>
+          <t xml:space="preserve">8451.64</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H82">
         <is>
-          <t xml:space="preserve">8784.10</t>
+          <t xml:space="preserve">8451.64</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I82">
@@ -3826,12 +3826,12 @@
       </c>
       <c s="9" t="inlineStr" r="J82">
         <is>
-          <t xml:space="preserve">8784.10</t>
+          <t xml:space="preserve">8451.64</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K82">
         <is>
-          <t xml:space="preserve">5900.23</t>
+          <t xml:space="preserve">4200.45</t>
         </is>
       </c>
     </row>
@@ -3847,22 +3847,22 @@
       </c>
       <c s="9" t="inlineStr" r="D83">
         <is>
-          <t xml:space="preserve">12204.60</t>
+          <t xml:space="preserve">9357.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F83">
         <is>
-          <t xml:space="preserve">8635.10</t>
+          <t xml:space="preserve">9237.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G83">
         <is>
-          <t xml:space="preserve">8443.10</t>
+          <t xml:space="preserve">7864.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H83">
         <is>
-          <t xml:space="preserve">8443.10</t>
+          <t xml:space="preserve">7864.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I83">
@@ -3872,12 +3872,12 @@
       </c>
       <c s="9" t="inlineStr" r="J83">
         <is>
-          <t xml:space="preserve">8443.10</t>
+          <t xml:space="preserve">7864.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K83">
         <is>
-          <t xml:space="preserve">7100.10</t>
+          <t xml:space="preserve">4098.59</t>
         </is>
       </c>
     </row>
@@ -3891,22 +3891,22 @@
       </c>
       <c s="9" t="inlineStr" r="D84">
         <is>
-          <t xml:space="preserve">12727.30</t>
+          <t xml:space="preserve">9152.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F84">
         <is>
-          <t xml:space="preserve">8574.30</t>
+          <t xml:space="preserve">8862.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G84">
         <is>
-          <t xml:space="preserve">8382.30</t>
+          <t xml:space="preserve">7619.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H84">
         <is>
-          <t xml:space="preserve">8382.30</t>
+          <t xml:space="preserve">7619.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I84">
@@ -3916,12 +3916,12 @@
       </c>
       <c s="9" t="inlineStr" r="J84">
         <is>
-          <t xml:space="preserve">8382.30</t>
+          <t xml:space="preserve">7619.60</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K84">
         <is>
-          <t xml:space="preserve">6505.11</t>
+          <t xml:space="preserve">4200.03</t>
         </is>
       </c>
     </row>
@@ -3935,22 +3935,22 @@
       </c>
       <c s="9" t="inlineStr" r="D85">
         <is>
-          <t xml:space="preserve">12656.30</t>
+          <t xml:space="preserve">9207.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F85">
         <is>
-          <t xml:space="preserve">8600.50</t>
+          <t xml:space="preserve">8684.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G85">
         <is>
-          <t xml:space="preserve">8333.50</t>
+          <t xml:space="preserve">7564.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H85">
         <is>
-          <t xml:space="preserve">8333.50</t>
+          <t xml:space="preserve">7564.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I85">
@@ -3960,12 +3960,12 @@
       </c>
       <c s="9" t="inlineStr" r="J85">
         <is>
-          <t xml:space="preserve">8333.50</t>
+          <t xml:space="preserve">7564.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K85">
         <is>
-          <t xml:space="preserve">5927.58</t>
+          <t xml:space="preserve">4399.01</t>
         </is>
       </c>
     </row>
@@ -3979,22 +3979,22 @@
       </c>
       <c s="9" t="inlineStr" r="D86">
         <is>
-          <t xml:space="preserve">12508.70</t>
+          <t xml:space="preserve">9101.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F86">
         <is>
-          <t xml:space="preserve">8660.50</t>
+          <t xml:space="preserve">8737.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G86">
         <is>
-          <t xml:space="preserve">8393.50</t>
+          <t xml:space="preserve">7512.68</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H86">
         <is>
-          <t xml:space="preserve">8393.50</t>
+          <t xml:space="preserve">7512.68</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I86">
@@ -4004,12 +4004,12 @@
       </c>
       <c s="9" t="inlineStr" r="J86">
         <is>
-          <t xml:space="preserve">8393.50</t>
+          <t xml:space="preserve">7512.68</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K86">
         <is>
-          <t xml:space="preserve">5893.94</t>
+          <t xml:space="preserve">4250.86</t>
         </is>
       </c>
     </row>
@@ -4025,22 +4025,22 @@
       </c>
       <c s="9" t="inlineStr" r="D87">
         <is>
-          <t xml:space="preserve">11418.30</t>
+          <t xml:space="preserve">8814.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F87">
         <is>
-          <t xml:space="preserve">8862.60</t>
+          <t xml:space="preserve">8837.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G87">
         <is>
-          <t xml:space="preserve">8497.00</t>
+          <t xml:space="preserve">7493.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H87">
         <is>
-          <t xml:space="preserve">8497.00</t>
+          <t xml:space="preserve">7493.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I87">
@@ -4050,12 +4050,12 @@
       </c>
       <c s="9" t="inlineStr" r="J87">
         <is>
-          <t xml:space="preserve">8497.00</t>
+          <t xml:space="preserve">7493.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K87">
         <is>
-          <t xml:space="preserve">5200.33</t>
+          <t xml:space="preserve">4098.40</t>
         </is>
       </c>
     </row>
@@ -4069,22 +4069,22 @@
       </c>
       <c s="9" t="inlineStr" r="D88">
         <is>
-          <t xml:space="preserve">10817.00</t>
+          <t xml:space="preserve">8889.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F88">
         <is>
-          <t xml:space="preserve">9067.60</t>
+          <t xml:space="preserve">8565.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G88">
         <is>
-          <t xml:space="preserve">8379.00</t>
+          <t xml:space="preserve">7470.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H88">
         <is>
-          <t xml:space="preserve">8379.00</t>
+          <t xml:space="preserve">7470.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I88">
@@ -4094,12 +4094,12 @@
       </c>
       <c s="9" t="inlineStr" r="J88">
         <is>
-          <t xml:space="preserve">8379.00</t>
+          <t xml:space="preserve">7470.40</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K88">
         <is>
-          <t xml:space="preserve">4960.05</t>
+          <t xml:space="preserve">4289.00</t>
         </is>
       </c>
     </row>
@@ -4113,22 +4113,22 @@
       </c>
       <c s="9" t="inlineStr" r="D89">
         <is>
-          <t xml:space="preserve">11460.30</t>
+          <t xml:space="preserve">9345.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F89">
         <is>
-          <t xml:space="preserve">8888.60</t>
+          <t xml:space="preserve">8465.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G89">
         <is>
-          <t xml:space="preserve">8523.00</t>
+          <t xml:space="preserve">7794.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H89">
         <is>
-          <t xml:space="preserve">8523.00</t>
+          <t xml:space="preserve">7794.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I89">
@@ -4138,12 +4138,12 @@
       </c>
       <c s="9" t="inlineStr" r="J89">
         <is>
-          <t xml:space="preserve">8523.00</t>
+          <t xml:space="preserve">7794.20</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K89">
         <is>
-          <t xml:space="preserve">5228.50</t>
+          <t xml:space="preserve">4600.19</t>
         </is>
       </c>
     </row>
@@ -4157,22 +4157,22 @@
       </c>
       <c s="9" t="inlineStr" r="D90">
         <is>
-          <t xml:space="preserve">12013.30</t>
+          <t xml:space="preserve">9900.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F90">
         <is>
-          <t xml:space="preserve">8727.10</t>
+          <t xml:space="preserve">8528.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G90">
         <is>
-          <t xml:space="preserve">8445.70</t>
+          <t xml:space="preserve">8162.37</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H90">
         <is>
-          <t xml:space="preserve">8445.70</t>
+          <t xml:space="preserve">8162.37</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I90">
@@ -4182,12 +4182,12 @@
       </c>
       <c s="9" t="inlineStr" r="J90">
         <is>
-          <t xml:space="preserve">8445.70</t>
+          <t xml:space="preserve">8162.37</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K90">
         <is>
-          <t xml:space="preserve">5536.31</t>
+          <t xml:space="preserve">4999.76</t>
         </is>
       </c>
     </row>
@@ -4203,22 +4203,22 @@
       </c>
       <c s="9" t="inlineStr" r="D91">
         <is>
-          <t xml:space="preserve">12324.00</t>
+          <t xml:space="preserve">10365.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F91">
         <is>
-          <t xml:space="preserve">8724.70</t>
+          <t xml:space="preserve">8371.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G91">
         <is>
-          <t xml:space="preserve">8442.90</t>
+          <t xml:space="preserve">8098.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H91">
         <is>
-          <t xml:space="preserve">8442.90</t>
+          <t xml:space="preserve">8098.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I91">
@@ -4228,12 +4228,12 @@
       </c>
       <c s="9" t="inlineStr" r="J91">
         <is>
-          <t xml:space="preserve">8442.90</t>
+          <t xml:space="preserve">8098.50</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K91">
         <is>
-          <t xml:space="preserve">5530.25</t>
+          <t xml:space="preserve">5000.29</t>
         </is>
       </c>
     </row>
@@ -4247,22 +4247,22 @@
       </c>
       <c s="9" t="inlineStr" r="D92">
         <is>
-          <t xml:space="preserve">12525.50</t>
+          <t xml:space="preserve">10711.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F92">
         <is>
-          <t xml:space="preserve">8800.70</t>
+          <t xml:space="preserve">8300.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G92">
         <is>
-          <t xml:space="preserve">8518.90</t>
+          <t xml:space="preserve">8013.86</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H92">
         <is>
-          <t xml:space="preserve">8518.90</t>
+          <t xml:space="preserve">8013.86</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I92">
@@ -4272,12 +4272,12 @@
       </c>
       <c s="9" t="inlineStr" r="J92">
         <is>
-          <t xml:space="preserve">8518.90</t>
+          <t xml:space="preserve">8013.86</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K92">
         <is>
-          <t xml:space="preserve">5586.75</t>
+          <t xml:space="preserve">5359.43</t>
         </is>
       </c>
     </row>
@@ -4291,22 +4291,22 @@
       </c>
       <c s="9" t="inlineStr" r="D93">
         <is>
-          <t xml:space="preserve">12463.30</t>
+          <t xml:space="preserve">10891.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F93">
         <is>
-          <t xml:space="preserve">9248.70</t>
+          <t xml:space="preserve">8642.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G93">
         <is>
-          <t xml:space="preserve">8882.70</t>
+          <t xml:space="preserve">8478.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H93">
         <is>
-          <t xml:space="preserve">8882.70</t>
+          <t xml:space="preserve">8478.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I93">
@@ -4316,12 +4316,12 @@
       </c>
       <c s="9" t="inlineStr" r="J93">
         <is>
-          <t xml:space="preserve">8882.70</t>
+          <t xml:space="preserve">8478.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K93">
         <is>
-          <t xml:space="preserve">5050.27</t>
+          <t xml:space="preserve">6000.35</t>
         </is>
       </c>
     </row>
@@ -4335,22 +4335,22 @@
       </c>
       <c s="9" t="inlineStr" r="D94">
         <is>
-          <t xml:space="preserve">12296.60</t>
+          <t xml:space="preserve">10511.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F94">
         <is>
-          <t xml:space="preserve">9821.10</t>
+          <t xml:space="preserve">8581.90</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G94">
         <is>
-          <t xml:space="preserve">9132.10</t>
+          <t xml:space="preserve">8339.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H94">
         <is>
-          <t xml:space="preserve">9132.10</t>
+          <t xml:space="preserve">8339.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I94">
@@ -4360,12 +4360,12 @@
       </c>
       <c s="9" t="inlineStr" r="J94">
         <is>
-          <t xml:space="preserve">9132.10</t>
+          <t xml:space="preserve">8339.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K94">
         <is>
-          <t xml:space="preserve">4810.45</t>
+          <t xml:space="preserve">5359.95</t>
         </is>
       </c>
     </row>
@@ -4381,22 +4381,22 @@
       </c>
       <c s="9" t="inlineStr" r="D95">
         <is>
-          <t xml:space="preserve">11625.40</t>
+          <t xml:space="preserve">10644.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F95">
         <is>
-          <t xml:space="preserve">10023.80</t>
+          <t xml:space="preserve">8592.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G95">
         <is>
-          <t xml:space="preserve">8840.63</t>
+          <t xml:space="preserve">8318.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H95">
         <is>
-          <t xml:space="preserve">8840.63</t>
+          <t xml:space="preserve">8318.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I95">
@@ -4406,12 +4406,12 @@
       </c>
       <c s="9" t="inlineStr" r="J95">
         <is>
-          <t xml:space="preserve">8840.63</t>
+          <t xml:space="preserve">8318.70</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K95">
         <is>
-          <t xml:space="preserve">4229.07</t>
+          <t xml:space="preserve">5000.54</t>
         </is>
       </c>
     </row>
@@ -4425,22 +4425,22 @@
       </c>
       <c s="9" t="inlineStr" r="D96">
         <is>
-          <t xml:space="preserve">11327.30</t>
+          <t xml:space="preserve">10766.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F96">
         <is>
-          <t xml:space="preserve">9904.70</t>
+          <t xml:space="preserve">8591.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G96">
         <is>
-          <t xml:space="preserve">8715.00</t>
+          <t xml:space="preserve">8353.23</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H96">
         <is>
-          <t xml:space="preserve">8715.00</t>
+          <t xml:space="preserve">8353.23</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I96">
@@ -4450,12 +4450,12 @@
       </c>
       <c s="9" t="inlineStr" r="J96">
         <is>
-          <t xml:space="preserve">8715.00</t>
+          <t xml:space="preserve">8353.23</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K96">
         <is>
-          <t xml:space="preserve">4203.20</t>
+          <t xml:space="preserve">5359.42</t>
         </is>
       </c>
     </row>
@@ -4469,22 +4469,22 @@
       </c>
       <c s="9" t="inlineStr" r="D97">
         <is>
-          <t xml:space="preserve">11111.50</t>
+          <t xml:space="preserve">10687.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F97">
         <is>
-          <t xml:space="preserve">9815.30</t>
+          <t xml:space="preserve">8242.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G97">
         <is>
-          <t xml:space="preserve">8600.80</t>
+          <t xml:space="preserve">8108.77</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H97">
         <is>
-          <t xml:space="preserve">8600.80</t>
+          <t xml:space="preserve">8108.77</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I97">
@@ -4494,12 +4494,12 @@
       </c>
       <c s="9" t="inlineStr" r="J97">
         <is>
-          <t xml:space="preserve">8600.80</t>
+          <t xml:space="preserve">8108.77</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K97">
         <is>
-          <t xml:space="preserve">4000.74</t>
+          <t xml:space="preserve">5999.12</t>
         </is>
       </c>
     </row>
@@ -4513,22 +4513,22 @@
       </c>
       <c s="9" t="inlineStr" r="D98">
         <is>
-          <t xml:space="preserve">11226.30</t>
+          <t xml:space="preserve">10489.50</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F98">
         <is>
-          <t xml:space="preserve">9554.00</t>
+          <t xml:space="preserve">8169.80</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G98">
         <is>
-          <t xml:space="preserve">8488.70</t>
+          <t xml:space="preserve">7980.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H98">
         <is>
-          <t xml:space="preserve">8488.70</t>
+          <t xml:space="preserve">7980.10</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I98">
@@ -4538,12 +4538,12 @@
       </c>
       <c s="9" t="inlineStr" r="J98">
         <is>
-          <t xml:space="preserve">8488.70</t>
+          <t xml:space="preserve">7980.10</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K98">
         <is>
-          <t xml:space="preserve">4340.38</t>
+          <t xml:space="preserve">5820.00</t>
         </is>
       </c>
     </row>
@@ -4559,22 +4559,22 @@
       </c>
       <c s="9" t="inlineStr" r="D99">
         <is>
-          <t xml:space="preserve">11811.50</t>
+          <t xml:space="preserve">10645.60</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F99">
         <is>
-          <t xml:space="preserve">9144.10</t>
+          <t xml:space="preserve">8346.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G99">
         <is>
-          <t xml:space="preserve">8709.40</t>
+          <t xml:space="preserve">8072.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H99">
         <is>
-          <t xml:space="preserve">8709.40</t>
+          <t xml:space="preserve">8072.40</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I99">
@@ -4584,12 +4584,12 @@
       </c>
       <c s="9" t="inlineStr" r="J99">
         <is>
-          <t xml:space="preserve">8709.40</t>
+          <t xml:space="preserve">8072.40</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K99">
         <is>
-          <t xml:space="preserve">4999.85</t>
+          <t xml:space="preserve">5000.08</t>
         </is>
       </c>
     </row>
@@ -4603,22 +4603,22 @@
       </c>
       <c s="9" t="inlineStr" r="D100">
         <is>
-          <t xml:space="preserve">11869.60</t>
+          <t xml:space="preserve">10307.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F100">
         <is>
-          <t xml:space="preserve">8800.40</t>
+          <t xml:space="preserve">8037.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G100">
         <is>
-          <t xml:space="preserve">8499.40</t>
+          <t xml:space="preserve">7732.64</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H100">
         <is>
-          <t xml:space="preserve">8499.40</t>
+          <t xml:space="preserve">7732.64</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I100">
@@ -4628,12 +4628,12 @@
       </c>
       <c s="9" t="inlineStr" r="J100">
         <is>
-          <t xml:space="preserve">8499.40</t>
+          <t xml:space="preserve">7732.64</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K100">
         <is>
-          <t xml:space="preserve">5410.20</t>
+          <t xml:space="preserve">4999.90</t>
         </is>
       </c>
     </row>
@@ -4647,22 +4647,22 @@
       </c>
       <c s="9" t="inlineStr" r="D101">
         <is>
-          <t xml:space="preserve">11683.80</t>
+          <t xml:space="preserve">9842.70</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F101">
         <is>
-          <t xml:space="preserve">8524.70</t>
+          <t xml:space="preserve">7810.00</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G101">
         <is>
-          <t xml:space="preserve">8051.60</t>
+          <t xml:space="preserve">7234.29</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H101">
         <is>
-          <t xml:space="preserve">8051.60</t>
+          <t xml:space="preserve">7234.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I101">
@@ -4672,12 +4672,12 @@
       </c>
       <c s="9" t="inlineStr" r="J101">
         <is>
-          <t xml:space="preserve">8051.60</t>
+          <t xml:space="preserve">7234.30</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K101">
         <is>
-          <t xml:space="preserve">4999.73</t>
+          <t xml:space="preserve">4999.07</t>
         </is>
       </c>
     </row>
@@ -4691,22 +4691,22 @@
       </c>
       <c s="9" t="inlineStr" r="D102">
         <is>
-          <t xml:space="preserve">11517.10</t>
+          <t xml:space="preserve">9218.20</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="F102">
         <is>
-          <t xml:space="preserve">8619.00</t>
+          <t xml:space="preserve">7416.30</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="G102">
         <is>
-          <t xml:space="preserve">8060.80</t>
+          <t xml:space="preserve">6582.37</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="H102">
         <is>
-          <t xml:space="preserve">8060.80</t>
+          <t xml:space="preserve">6582.37</t>
         </is>
       </c>
       <c s="9" t="inlineStr" r="I102">
@@ -4716,12 +4716,12 @@
       </c>
       <c s="9" t="inlineStr" r="J102">
         <is>
-          <t xml:space="preserve">8060.80</t>
+          <t xml:space="preserve">6582.37</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K102">
         <is>
-          <t xml:space="preserve">4999.46</t>
+          <t xml:space="preserve">4475.86</t>
         </is>
       </c>
     </row>
@@ -4796,7 +4796,7 @@
     <row r="105" ht="15" customHeight="0">
       <c s="6" t="inlineStr" r="A105">
         <is>
-          <t xml:space="preserve">05-04-2021</t>
+          <t xml:space="preserve">14-04-2021</t>
         </is>
       </c>
       <c s="16" t="inlineStr" r="B105">
@@ -4807,22 +4807,22 @@
       <c s="5" t="str" r="C105"/>
       <c s="17" t="inlineStr" r="D105">
         <is>
-          <t xml:space="preserve">295420.15</t>
+          <t xml:space="preserve">219301.13</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="F105">
         <is>
-          <t xml:space="preserve">282736.00</t>
+          <t xml:space="preserve">258741.15</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="G105">
         <is>
-          <t xml:space="preserve">238261.29</t>
+          <t xml:space="preserve">182912.37</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="H105">
         <is>
-          <t xml:space="preserve">238261.30</t>
+          <t xml:space="preserve">182912.38</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="I105">
@@ -4832,7 +4832,7 @@
       </c>
       <c s="17" t="inlineStr" r="J105">
         <is>
-          <t xml:space="preserve">238261.30</t>
+          <t xml:space="preserve">182912.38</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K105">
@@ -4851,22 +4851,22 @@
       <c s="5" t="str" r="C106"/>
       <c s="17" t="inlineStr" r="D106">
         <is>
-          <t xml:space="preserve">15371.70</t>
+          <t xml:space="preserve">11600.60</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="F106">
         <is>
-          <t xml:space="preserve">16460.40</t>
+          <t xml:space="preserve">15553.50</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="G106">
         <is>
-          <t xml:space="preserve">12027.90</t>
+          <t xml:space="preserve">10013.06</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="H106">
         <is>
-          <t xml:space="preserve">12027.90</t>
+          <t xml:space="preserve">10013.06</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="I106">
@@ -4876,12 +4876,12 @@
       </c>
       <c s="17" t="inlineStr" r="J106">
         <is>
-          <t xml:space="preserve">12027.90</t>
+          <t xml:space="preserve">10013.06</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K106">
         <is>
-          <t xml:space="preserve">7100.10</t>
+          <t xml:space="preserve">6500.10</t>
         </is>
       </c>
     </row>
@@ -4895,22 +4895,22 @@
       <c s="5" t="str" r="C107"/>
       <c s="17" t="inlineStr" r="D107">
         <is>
-          <t xml:space="preserve">10635.90</t>
+          <t xml:space="preserve">7009.50</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="F107">
         <is>
-          <t xml:space="preserve">8524.70</t>
+          <t xml:space="preserve">6615.50</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="G107">
         <is>
-          <t xml:space="preserve">8051.60</t>
+          <t xml:space="preserve">5746.12</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="H107">
         <is>
-          <t xml:space="preserve">8051.60</t>
+          <t xml:space="preserve">5746.12</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="I107">
@@ -4920,12 +4920,12 @@
       </c>
       <c s="17" t="inlineStr" r="J107">
         <is>
-          <t xml:space="preserve">8051.60</t>
+          <t xml:space="preserve">5746.12</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K107">
         <is>
-          <t xml:space="preserve">2979.47</t>
+          <t xml:space="preserve">2546.50</t>
         </is>
       </c>
     </row>
@@ -4939,22 +4939,22 @@
       <c s="5" t="str" r="C108"/>
       <c s="17" t="inlineStr" r="D108">
         <is>
-          <t xml:space="preserve">12309.17</t>
+          <t xml:space="preserve">9137.55</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="F108">
         <is>
-          <t xml:space="preserve">11780.67</t>
+          <t xml:space="preserve">10780.88</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="G108">
         <is>
-          <t xml:space="preserve">9927.55</t>
+          <t xml:space="preserve">7621.35</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="H108">
         <is>
-          <t xml:space="preserve">9927.55</t>
+          <t xml:space="preserve">7621.35</t>
         </is>
       </c>
       <c s="17" t="inlineStr" r="I108">
@@ -4964,12 +4964,12 @@
       </c>
       <c s="17" t="inlineStr" r="J108">
         <is>
-          <t xml:space="preserve">9927.55</t>
+          <t xml:space="preserve">7621.35</t>
         </is>
       </c>
       <c s="10" t="inlineStr" r="K108">
         <is>
-          <t xml:space="preserve">4140.40</t>
+          <t xml:space="preserve">3793.49</t>
         </is>
       </c>
     </row>

</xml_diff>